<commit_message>
Fixed print canonical type
</commit_message>
<xml_diff>
--- a/material/translation/DomicileRegistrationEvidence/MOR2_ro_en_es_sl_pt_fr.xlsx
+++ b/material/translation/DomicileRegistrationEvidence/MOR2_ro_en_es_sl_pt_fr.xlsx
@@ -331,9 +331,6 @@
     <t>La région de l'adresse, généralement un comté, un État ou un autre domaine de ce type qui englobe généralement plusieurs localités.</t>
   </si>
   <si>
-    <t>CountryEnum</t>
-  </si>
-  <si>
     <t>Unitate administrativă nivel 1</t>
   </si>
   <si>
@@ -1842,6 +1839,9 @@
   </si>
   <si>
     <t>L'ID d'agence émettrice</t>
+  </si>
+  <si>
+    <t>CountryEnum</t>
   </si>
   <si>
     <t>http://publications.europa.eu/resource/authority/country/</t>
@@ -10777,70 +10777,70 @@
         <v>67</v>
       </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="17" t="s">
-        <v>106</v>
+      <c r="C14" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>107</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>108</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="19">
         <v>1.0</v>
       </c>
       <c r="J14" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="K14" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="L14" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="M14" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="N14" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="N14" s="17" t="s">
+      <c r="O14" s="17" t="s">
         <v>112</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>113</v>
       </c>
       <c r="P14" s="18"/>
       <c r="Q14" s="19">
         <v>1.0</v>
       </c>
       <c r="R14" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="S14" s="17" t="s">
         <v>114</v>
-      </c>
-      <c r="S14" s="17" t="s">
-        <v>115</v>
       </c>
       <c r="T14" s="18"/>
       <c r="U14" s="19">
         <v>1.0</v>
       </c>
       <c r="V14" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="W14" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="W14" s="17" t="s">
-        <v>117</v>
       </c>
       <c r="X14" s="18"/>
       <c r="Y14" s="19">
         <v>1.0</v>
       </c>
       <c r="Z14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA14" s="17" t="s">
         <v>118</v>
-      </c>
-      <c r="AA14" s="17" t="s">
-        <v>119</v>
       </c>
       <c r="AB14" s="15"/>
       <c r="AC14" s="20">
@@ -10849,10 +10849,10 @@
     </row>
     <row r="15">
       <c r="A15" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>121</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>92</v>
@@ -10862,20 +10862,20 @@
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>122</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>123</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="25">
         <v>1.0</v>
       </c>
       <c r="J15" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="K15" s="22" t="s">
         <v>124</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>125</v>
       </c>
       <c r="L15" s="22">
         <v>28045.0</v>
@@ -10884,40 +10884,40 @@
         <v>1.0</v>
       </c>
       <c r="N15" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="O15" s="22" t="s">
         <v>126</v>
-      </c>
-      <c r="O15" s="22" t="s">
-        <v>127</v>
       </c>
       <c r="P15" s="24"/>
       <c r="Q15" s="25">
         <v>1.0</v>
       </c>
       <c r="R15" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="S15" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="S15" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="T15" s="24"/>
       <c r="U15" s="25">
         <v>1.0</v>
       </c>
       <c r="V15" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="W15" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="W15" s="22" t="s">
-        <v>131</v>
       </c>
       <c r="X15" s="24"/>
       <c r="Y15" s="25">
         <v>1.0</v>
       </c>
       <c r="Z15" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA15" s="22" t="s">
         <v>132</v>
-      </c>
-      <c r="AA15" s="22" t="s">
-        <v>133</v>
       </c>
       <c r="AB15" s="26"/>
       <c r="AC15" s="27">
@@ -10926,10 +10926,10 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>135</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>92</v>
@@ -10939,62 +10939,62 @@
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>137</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="19">
         <v>1.0</v>
       </c>
       <c r="J16" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K16" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="L16" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="M16" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="N16" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="M16" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="N16" s="17" t="s">
+      <c r="O16" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>142</v>
       </c>
       <c r="P16" s="18"/>
       <c r="Q16" s="19">
         <v>1.0</v>
       </c>
       <c r="R16" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="S16" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="S16" s="17" t="s">
-        <v>144</v>
       </c>
       <c r="T16" s="18"/>
       <c r="U16" s="19">
         <v>1.0</v>
       </c>
       <c r="V16" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="W16" s="17" t="s">
         <v>145</v>
-      </c>
-      <c r="W16" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="X16" s="18"/>
       <c r="Y16" s="19">
         <v>1.0</v>
       </c>
       <c r="Z16" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA16" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="AA16" s="17" t="s">
-        <v>148</v>
       </c>
       <c r="AB16" s="15"/>
       <c r="AC16" s="20">
@@ -11003,10 +11003,10 @@
     </row>
     <row r="17">
       <c r="A17" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>149</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>150</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>92</v>
@@ -11016,62 +11016,62 @@
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="22" t="s">
         <v>151</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>152</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="25">
         <v>1.0</v>
       </c>
       <c r="J17" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K17" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="L17" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="M17" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="N17" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="M17" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="N17" s="22" t="s">
+      <c r="O17" s="22" t="s">
         <v>156</v>
-      </c>
-      <c r="O17" s="22" t="s">
-        <v>157</v>
       </c>
       <c r="P17" s="24"/>
       <c r="Q17" s="25">
         <v>1.0</v>
       </c>
       <c r="R17" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="S17" s="22" t="s">
         <v>158</v>
-      </c>
-      <c r="S17" s="22" t="s">
-        <v>159</v>
       </c>
       <c r="T17" s="24"/>
       <c r="U17" s="25">
         <v>1.0</v>
       </c>
       <c r="V17" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="W17" s="22" t="s">
         <v>160</v>
-      </c>
-      <c r="W17" s="22" t="s">
-        <v>161</v>
       </c>
       <c r="X17" s="24"/>
       <c r="Y17" s="25">
         <v>1.0</v>
       </c>
       <c r="Z17" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA17" s="22" t="s">
         <v>162</v>
-      </c>
-      <c r="AA17" s="22" t="s">
-        <v>163</v>
       </c>
       <c r="AB17" s="26"/>
       <c r="AC17" s="27">
@@ -11080,10 +11080,10 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>92</v>
@@ -11093,62 +11093,62 @@
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>167</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="19">
         <v>1.0</v>
       </c>
       <c r="J18" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="K18" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="L18" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="M18" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="N18" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="M18" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="N18" s="17" t="s">
+      <c r="O18" s="17" t="s">
         <v>171</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>172</v>
       </c>
       <c r="P18" s="18"/>
       <c r="Q18" s="19">
         <v>1.0</v>
       </c>
       <c r="R18" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="S18" s="17" t="s">
         <v>173</v>
-      </c>
-      <c r="S18" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="T18" s="18"/>
       <c r="U18" s="19">
         <v>1.0</v>
       </c>
       <c r="V18" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="W18" s="17" t="s">
         <v>175</v>
-      </c>
-      <c r="W18" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="X18" s="18"/>
       <c r="Y18" s="19">
         <v>1.0</v>
       </c>
       <c r="Z18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA18" s="17" t="s">
         <v>177</v>
-      </c>
-      <c r="AA18" s="17" t="s">
-        <v>178</v>
       </c>
       <c r="AB18" s="15"/>
       <c r="AC18" s="20">
@@ -11157,10 +11157,10 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>179</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>180</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>92</v>
@@ -11170,20 +11170,20 @@
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="G19" s="22" t="s">
         <v>181</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>182</v>
       </c>
       <c r="H19" s="24"/>
       <c r="I19" s="25">
         <v>1.0</v>
       </c>
       <c r="J19" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="K19" s="22" t="s">
         <v>183</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>184</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>97</v>
@@ -11192,40 +11192,40 @@
         <v>1.0</v>
       </c>
       <c r="N19" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="O19" s="22" t="s">
         <v>185</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>186</v>
       </c>
       <c r="P19" s="24"/>
       <c r="Q19" s="25">
         <v>1.0</v>
       </c>
       <c r="R19" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="S19" s="22" t="s">
         <v>187</v>
-      </c>
-      <c r="S19" s="22" t="s">
-        <v>188</v>
       </c>
       <c r="T19" s="24"/>
       <c r="U19" s="25">
         <v>1.0</v>
       </c>
       <c r="V19" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="W19" s="22" t="s">
         <v>189</v>
-      </c>
-      <c r="W19" s="22" t="s">
-        <v>190</v>
       </c>
       <c r="X19" s="24"/>
       <c r="Y19" s="25">
         <v>1.0</v>
       </c>
       <c r="Z19" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA19" s="22" t="s">
         <v>191</v>
-      </c>
-      <c r="AA19" s="22" t="s">
-        <v>192</v>
       </c>
       <c r="AB19" s="26"/>
       <c r="AC19" s="27">
@@ -11234,10 +11234,10 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>193</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>194</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>92</v>
@@ -11247,20 +11247,20 @@
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>195</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>196</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="19">
         <v>1.0</v>
       </c>
       <c r="J20" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="K20" s="17" t="s">
         <v>197</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>198</v>
       </c>
       <c r="L20" s="17" t="s">
         <v>97</v>
@@ -11269,40 +11269,40 @@
         <v>1.0</v>
       </c>
       <c r="N20" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="O20" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="O20" s="17" t="s">
-        <v>200</v>
       </c>
       <c r="P20" s="18"/>
       <c r="Q20" s="19">
         <v>1.0</v>
       </c>
       <c r="R20" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="S20" s="17" t="s">
         <v>201</v>
-      </c>
-      <c r="S20" s="17" t="s">
-        <v>202</v>
       </c>
       <c r="T20" s="18"/>
       <c r="U20" s="19">
         <v>1.0</v>
       </c>
       <c r="V20" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="W20" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X20" s="18"/>
       <c r="Y20" s="19">
         <v>1.0</v>
       </c>
       <c r="Z20" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA20" s="17" t="s">
         <v>204</v>
-      </c>
-      <c r="AA20" s="17" t="s">
-        <v>205</v>
       </c>
       <c r="AB20" s="15"/>
       <c r="AC20" s="20">
@@ -11311,10 +11311,10 @@
     </row>
     <row r="21">
       <c r="A21" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>206</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>207</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>92</v>
@@ -11324,62 +11324,62 @@
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="G21" s="22" t="s">
         <v>208</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>209</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="25">
         <v>1.0</v>
       </c>
       <c r="J21" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="K21" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="L21" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="M21" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="N21" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="M21" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="N21" s="22" t="s">
+      <c r="O21" s="22" t="s">
         <v>213</v>
-      </c>
-      <c r="O21" s="22" t="s">
-        <v>214</v>
       </c>
       <c r="P21" s="24"/>
       <c r="Q21" s="25">
         <v>1.0</v>
       </c>
       <c r="R21" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="S21" s="22" t="s">
         <v>215</v>
-      </c>
-      <c r="S21" s="22" t="s">
-        <v>216</v>
       </c>
       <c r="T21" s="24"/>
       <c r="U21" s="25">
         <v>1.0</v>
       </c>
       <c r="V21" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W21" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="25">
         <v>1.0</v>
       </c>
       <c r="Z21" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA21" s="22" t="s">
         <v>218</v>
-      </c>
-      <c r="AA21" s="22" t="s">
-        <v>219</v>
       </c>
       <c r="AB21" s="26"/>
       <c r="AC21" s="27">
@@ -11395,10 +11395,10 @@
       <c r="D22" s="16"/>
       <c r="E22" s="15"/>
       <c r="F22" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>220</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>221</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="19">
@@ -11408,14 +11408,14 @@
         <v>74</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L22" s="15"/>
       <c r="M22" s="19">
         <v>1.0</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O22" s="18"/>
       <c r="P22" s="18"/>
@@ -11423,17 +11423,17 @@
         <v>1.0</v>
       </c>
       <c r="R22" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="S22" s="17" t="s">
         <v>224</v>
-      </c>
-      <c r="S22" s="17" t="s">
-        <v>225</v>
       </c>
       <c r="T22" s="15"/>
       <c r="U22" s="19">
         <v>1.0</v>
       </c>
       <c r="V22" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W22" s="18"/>
       <c r="X22" s="15"/>
@@ -11441,7 +11441,7 @@
         <v>1.0</v>
       </c>
       <c r="Z22" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AA22" s="15"/>
       <c r="AB22" s="15"/>
@@ -11451,7 +11451,7 @@
     </row>
     <row r="23">
       <c r="A23" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="24"/>
@@ -11460,27 +11460,27 @@
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>229</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>230</v>
       </c>
       <c r="H23" s="24"/>
       <c r="I23" s="25">
         <v>1.0</v>
       </c>
       <c r="J23" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="K23" s="22" t="s">
         <v>231</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>232</v>
       </c>
       <c r="L23" s="26"/>
       <c r="M23" s="25">
         <v>1.0</v>
       </c>
       <c r="N23" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O23" s="24"/>
       <c r="P23" s="24"/>
@@ -11488,17 +11488,17 @@
         <v>1.0</v>
       </c>
       <c r="R23" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="S23" s="22" t="s">
         <v>234</v>
-      </c>
-      <c r="S23" s="22" t="s">
-        <v>235</v>
       </c>
       <c r="T23" s="26"/>
       <c r="U23" s="25">
         <v>1.0</v>
       </c>
       <c r="V23" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="W23" s="24"/>
       <c r="X23" s="26"/>
@@ -11506,7 +11506,7 @@
         <v>1.0</v>
       </c>
       <c r="Z23" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA23" s="26"/>
       <c r="AB23" s="26"/>
@@ -11516,31 +11516,31 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>240</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>241</v>
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="19">
         <v>1.0</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="K24" s="17" t="s">
         <v>242</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>243</v>
       </c>
       <c r="L24" s="17">
         <v>1980.0</v>
@@ -11549,7 +11549,7 @@
         <v>1.0</v>
       </c>
       <c r="N24" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
@@ -11557,17 +11557,17 @@
         <v>1.0</v>
       </c>
       <c r="R24" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="S24" s="17" t="s">
         <v>245</v>
-      </c>
-      <c r="S24" s="17" t="s">
-        <v>246</v>
       </c>
       <c r="T24" s="15"/>
       <c r="U24" s="19">
         <v>1.0</v>
       </c>
       <c r="V24" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="W24" s="18"/>
       <c r="X24" s="15"/>
@@ -11575,7 +11575,7 @@
         <v>1.0</v>
       </c>
       <c r="Z24" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AA24" s="15"/>
       <c r="AB24" s="15"/>
@@ -11585,31 +11585,31 @@
     </row>
     <row r="25">
       <c r="A25" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>250</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>251</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25">
         <v>1.0</v>
       </c>
       <c r="J25" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="K25" s="22" t="s">
         <v>252</v>
-      </c>
-      <c r="K25" s="22" t="s">
-        <v>253</v>
       </c>
       <c r="L25" s="22">
         <v>6.0</v>
@@ -11618,7 +11618,7 @@
         <v>1.0</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
@@ -11626,17 +11626,17 @@
         <v>1.0</v>
       </c>
       <c r="R25" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="S25" s="22" t="s">
         <v>255</v>
-      </c>
-      <c r="S25" s="22" t="s">
-        <v>256</v>
       </c>
       <c r="T25" s="26"/>
       <c r="U25" s="25">
         <v>1.0</v>
       </c>
       <c r="V25" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="W25" s="24"/>
       <c r="X25" s="26"/>
@@ -11644,7 +11644,7 @@
         <v>1.0</v>
       </c>
       <c r="Z25" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AA25" s="26"/>
       <c r="AB25" s="26"/>
@@ -11654,31 +11654,31 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D26" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>261</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>262</v>
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="19">
         <v>1.0</v>
       </c>
       <c r="J26" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="K26" s="17" t="s">
         <v>263</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>264</v>
       </c>
       <c r="L26" s="17">
         <v>12.0</v>
@@ -11687,7 +11687,7 @@
         <v>1.0</v>
       </c>
       <c r="N26" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O26" s="18"/>
       <c r="P26" s="18"/>
@@ -11695,17 +11695,17 @@
         <v>1.0</v>
       </c>
       <c r="R26" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="S26" s="17" t="s">
         <v>266</v>
-      </c>
-      <c r="S26" s="17" t="s">
-        <v>267</v>
       </c>
       <c r="T26" s="15"/>
       <c r="U26" s="19">
         <v>1.0</v>
       </c>
       <c r="V26" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W26" s="18"/>
       <c r="X26" s="15"/>
@@ -11713,7 +11713,7 @@
         <v>1.0</v>
       </c>
       <c r="Z26" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA26" s="15"/>
       <c r="AB26" s="15"/>
@@ -11723,40 +11723,40 @@
     </row>
     <row r="27">
       <c r="A27" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="G27" s="22" t="s">
         <v>272</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>273</v>
       </c>
       <c r="H27" s="24"/>
       <c r="I27" s="25">
         <v>1.0</v>
       </c>
       <c r="J27" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="K27" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="K27" s="22" t="s">
+      <c r="L27" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="L27" s="22" t="s">
+      <c r="M27" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="N27" s="22" t="s">
         <v>276</v>
-      </c>
-      <c r="M27" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="N27" s="22" t="s">
-        <v>277</v>
       </c>
       <c r="O27" s="24"/>
       <c r="P27" s="24"/>
@@ -11764,17 +11764,17 @@
         <v>1.0</v>
       </c>
       <c r="R27" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="S27" s="22" t="s">
         <v>278</v>
-      </c>
-      <c r="S27" s="22" t="s">
-        <v>279</v>
       </c>
       <c r="T27" s="26"/>
       <c r="U27" s="25">
         <v>1.0</v>
       </c>
       <c r="V27" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="W27" s="24"/>
       <c r="X27" s="26"/>
@@ -11782,7 +11782,7 @@
         <v>1.0</v>
       </c>
       <c r="Z27" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AA27" s="26"/>
       <c r="AB27" s="26"/>
@@ -11792,7 +11792,7 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="17" t="s">
@@ -11803,27 +11803,27 @@
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="G28" s="17" t="s">
         <v>282</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>283</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="19">
         <v>1.0</v>
       </c>
       <c r="J28" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="K28" s="17" t="s">
         <v>284</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>285</v>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="19">
         <v>1.0</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O28" s="18"/>
       <c r="P28" s="18"/>
@@ -11831,17 +11831,17 @@
         <v>1.0</v>
       </c>
       <c r="R28" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="S28" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="S28" s="17" t="s">
-        <v>288</v>
       </c>
       <c r="T28" s="15"/>
       <c r="U28" s="19">
         <v>1.0</v>
       </c>
       <c r="V28" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W28" s="18"/>
       <c r="X28" s="15"/>
@@ -11849,7 +11849,7 @@
         <v>1.0</v>
       </c>
       <c r="Z28" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AA28" s="15"/>
       <c r="AB28" s="15"/>
@@ -11859,7 +11859,7 @@
     </row>
     <row r="29">
       <c r="A29" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="24"/>
@@ -11868,27 +11868,27 @@
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="G29" s="22" t="s">
         <v>292</v>
-      </c>
-      <c r="G29" s="22" t="s">
-        <v>293</v>
       </c>
       <c r="H29" s="24"/>
       <c r="I29" s="25">
         <v>1.0</v>
       </c>
       <c r="J29" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="K29" s="22" t="s">
         <v>294</v>
-      </c>
-      <c r="K29" s="22" t="s">
-        <v>295</v>
       </c>
       <c r="L29" s="26"/>
       <c r="M29" s="25">
         <v>1.0</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
@@ -11896,17 +11896,17 @@
         <v>1.0</v>
       </c>
       <c r="R29" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="S29" s="22" t="s">
         <v>297</v>
-      </c>
-      <c r="S29" s="22" t="s">
-        <v>298</v>
       </c>
       <c r="T29" s="26"/>
       <c r="U29" s="25">
         <v>1.0</v>
       </c>
       <c r="V29" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="W29" s="24"/>
       <c r="X29" s="26"/>
@@ -11914,7 +11914,7 @@
         <v>1.0</v>
       </c>
       <c r="Z29" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AA29" s="26"/>
       <c r="AB29" s="26"/>
@@ -11924,42 +11924,42 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="D30" s="28" t="s">
         <v>303</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>304</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>305</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>306</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="19">
         <v>1.0</v>
       </c>
       <c r="J30" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="K30" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="K30" s="17" t="s">
+      <c r="L30" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="L30" s="17" t="s">
+      <c r="M30" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="N30" s="17" t="s">
         <v>309</v>
-      </c>
-      <c r="M30" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="N30" s="17" t="s">
-        <v>310</v>
       </c>
       <c r="O30" s="18"/>
       <c r="P30" s="18"/>
@@ -11967,17 +11967,17 @@
         <v>1.0</v>
       </c>
       <c r="R30" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="S30" s="17" t="s">
         <v>311</v>
-      </c>
-      <c r="S30" s="17" t="s">
-        <v>312</v>
       </c>
       <c r="T30" s="15"/>
       <c r="U30" s="19">
         <v>1.0</v>
       </c>
       <c r="V30" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="W30" s="18"/>
       <c r="X30" s="15"/>
@@ -11985,7 +11985,7 @@
         <v>1.0</v>
       </c>
       <c r="Z30" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AA30" s="15"/>
       <c r="AB30" s="15"/>
@@ -11995,42 +11995,42 @@
     </row>
     <row r="31">
       <c r="A31" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>315</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>316</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>92</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="G31" s="22" t="s">
         <v>317</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>318</v>
       </c>
       <c r="H31" s="24"/>
       <c r="I31" s="25">
         <v>1.0</v>
       </c>
       <c r="J31" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="K31" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="L31" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="L31" s="22" t="s">
+      <c r="M31" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="N31" s="22" t="s">
         <v>321</v>
-      </c>
-      <c r="M31" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="N31" s="22" t="s">
-        <v>322</v>
       </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
@@ -12038,17 +12038,17 @@
         <v>1.0</v>
       </c>
       <c r="R31" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="S31" s="22" t="s">
         <v>323</v>
-      </c>
-      <c r="S31" s="22" t="s">
-        <v>324</v>
       </c>
       <c r="T31" s="26"/>
       <c r="U31" s="25">
         <v>1.0</v>
       </c>
       <c r="V31" s="22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="W31" s="24"/>
       <c r="X31" s="26"/>
@@ -12056,7 +12056,7 @@
         <v>1.0</v>
       </c>
       <c r="Z31" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AA31" s="26"/>
       <c r="AB31" s="26"/>
@@ -12066,21 +12066,21 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="G32" s="17" t="s">
         <v>328</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>329</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="19">
@@ -12090,7 +12090,7 @@
         <v>36</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L32" s="15"/>
       <c r="M32" s="19">
@@ -12105,10 +12105,10 @@
         <v>1.0</v>
       </c>
       <c r="R32" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="S32" s="17" t="s">
         <v>331</v>
-      </c>
-      <c r="S32" s="17" t="s">
-        <v>332</v>
       </c>
       <c r="T32" s="15"/>
       <c r="U32" s="19">
@@ -12123,7 +12123,7 @@
         <v>1.0</v>
       </c>
       <c r="Z32" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA32" s="15"/>
       <c r="AB32" s="15"/>
@@ -12133,38 +12133,38 @@
     </row>
     <row r="33">
       <c r="A33" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="G33" s="22" t="s">
         <v>336</v>
-      </c>
-      <c r="G33" s="22" t="s">
-        <v>337</v>
       </c>
       <c r="H33" s="24"/>
       <c r="I33" s="25">
         <v>1.0</v>
       </c>
       <c r="J33" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="K33" s="22" t="s">
         <v>338</v>
-      </c>
-      <c r="K33" s="22" t="s">
-        <v>339</v>
       </c>
       <c r="L33" s="26"/>
       <c r="M33" s="25">
         <v>1.0</v>
       </c>
       <c r="N33" s="22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="O33" s="24"/>
       <c r="P33" s="24"/>
@@ -12172,17 +12172,17 @@
         <v>1.0</v>
       </c>
       <c r="R33" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="S33" s="22" t="s">
         <v>341</v>
-      </c>
-      <c r="S33" s="22" t="s">
-        <v>342</v>
       </c>
       <c r="T33" s="26"/>
       <c r="U33" s="25">
         <v>1.0</v>
       </c>
       <c r="V33" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="W33" s="24"/>
       <c r="X33" s="26"/>
@@ -12190,7 +12190,7 @@
         <v>1.0</v>
       </c>
       <c r="Z33" s="22" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AA33" s="26"/>
       <c r="AB33" s="26"/>
@@ -12207,7 +12207,7 @@
       <c r="D34" s="30"/>
       <c r="E34" s="15"/>
       <c r="F34" s="17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -12223,7 +12223,7 @@
         <v>1.0</v>
       </c>
       <c r="N34" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
@@ -12237,7 +12237,7 @@
         <v>1.0</v>
       </c>
       <c r="V34" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="W34" s="15"/>
       <c r="X34" s="15"/>
@@ -12245,7 +12245,7 @@
         <v>1.0</v>
       </c>
       <c r="Z34" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AA34" s="15"/>
       <c r="AB34" s="15"/>
@@ -12255,21 +12255,21 @@
     </row>
     <row r="35">
       <c r="A35" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="25">
@@ -12279,7 +12279,7 @@
         <v>36</v>
       </c>
       <c r="K35" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L35" s="26"/>
       <c r="M35" s="22">
@@ -12289,17 +12289,17 @@
         <v>40</v>
       </c>
       <c r="O35" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P35" s="26"/>
       <c r="Q35" s="22">
         <v>1.0</v>
       </c>
       <c r="R35" s="22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S35" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T35" s="26"/>
       <c r="U35" s="22">
@@ -12309,17 +12309,17 @@
         <v>40</v>
       </c>
       <c r="W35" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="X35" s="26"/>
       <c r="Y35" s="22">
         <v>1.0</v>
       </c>
       <c r="Z35" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA35" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AB35" s="26"/>
       <c r="AC35" s="32">
@@ -12328,10 +12328,10 @@
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>356</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>357</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>92</v>
@@ -12341,62 +12341,62 @@
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="G36" s="17" t="s">
         <v>358</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>359</v>
       </c>
       <c r="H36" s="15"/>
       <c r="I36" s="19">
         <v>1.0</v>
       </c>
       <c r="J36" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="K36" s="17" t="s">
         <v>360</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="L36" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="L36" s="17" t="s">
+      <c r="M36" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="N36" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="M36" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="N36" s="17" t="s">
+      <c r="O36" s="17" t="s">
         <v>363</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>364</v>
       </c>
       <c r="P36" s="15"/>
       <c r="Q36" s="17">
         <v>1.0</v>
       </c>
       <c r="R36" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="S36" s="17" t="s">
         <v>365</v>
-      </c>
-      <c r="S36" s="17" t="s">
-        <v>366</v>
       </c>
       <c r="T36" s="15"/>
       <c r="U36" s="17">
         <v>1.0</v>
       </c>
       <c r="V36" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="W36" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="X36" s="15"/>
       <c r="Y36" s="17">
         <v>1.0</v>
       </c>
       <c r="Z36" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="AA36" s="17" t="s">
         <v>368</v>
-      </c>
-      <c r="AA36" s="17" t="s">
-        <v>369</v>
       </c>
       <c r="AB36" s="15"/>
       <c r="AC36" s="31">
@@ -12405,7 +12405,7 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>30</v>
@@ -12455,10 +12455,10 @@
         <v>92</v>
       </c>
       <c r="B38" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>371</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>372</v>
       </c>
       <c r="D38" s="23" t="s">
         <v>37</v>
@@ -12467,62 +12467,62 @@
         <v>45</v>
       </c>
       <c r="F38" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="G38" s="22" t="s">
         <v>373</v>
-      </c>
-      <c r="G38" s="22" t="s">
-        <v>374</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="25">
         <v>1.0</v>
       </c>
       <c r="J38" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K38" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="L38" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="L38" s="22" t="s">
+      <c r="M38" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="N38" s="22" t="s">
         <v>376</v>
       </c>
-      <c r="M38" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="N38" s="22" t="s">
+      <c r="O38" s="22" t="s">
         <v>377</v>
-      </c>
-      <c r="O38" s="22" t="s">
-        <v>378</v>
       </c>
       <c r="P38" s="26"/>
       <c r="Q38" s="25">
         <v>1.0</v>
       </c>
       <c r="R38" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="S38" s="22" t="s">
         <v>379</v>
-      </c>
-      <c r="S38" s="22" t="s">
-        <v>380</v>
       </c>
       <c r="T38" s="26"/>
       <c r="U38" s="25">
         <v>1.0</v>
       </c>
       <c r="V38" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="W38" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="X38" s="26"/>
       <c r="Y38" s="25">
         <v>1.0</v>
       </c>
       <c r="Z38" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="AA38" s="22" t="s">
         <v>382</v>
-      </c>
-      <c r="AA38" s="22" t="s">
-        <v>383</v>
       </c>
       <c r="AB38" s="26"/>
       <c r="AC38" s="27">
@@ -12531,73 +12531,73 @@
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>384</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>385</v>
       </c>
       <c r="D39" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="G39" s="17" t="s">
         <v>386</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>387</v>
       </c>
       <c r="H39" s="15"/>
       <c r="I39" s="19">
         <v>1.0</v>
       </c>
       <c r="J39" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="K39" s="17" t="s">
         <v>388</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>389</v>
       </c>
       <c r="L39" s="15"/>
       <c r="M39" s="19">
         <v>1.0</v>
       </c>
       <c r="N39" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="O39" s="17" t="s">
         <v>390</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>391</v>
       </c>
       <c r="P39" s="15"/>
       <c r="Q39" s="19">
         <v>1.0</v>
       </c>
       <c r="R39" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="S39" s="17" t="s">
         <v>392</v>
-      </c>
-      <c r="S39" s="17" t="s">
-        <v>393</v>
       </c>
       <c r="T39" s="15"/>
       <c r="U39" s="19">
         <v>1.0</v>
       </c>
       <c r="V39" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="W39" s="17" t="s">
         <v>394</v>
-      </c>
-      <c r="W39" s="17" t="s">
-        <v>395</v>
       </c>
       <c r="X39" s="15"/>
       <c r="Y39" s="19">
         <v>1.0</v>
       </c>
       <c r="Z39" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="AA39" s="17" t="s">
         <v>396</v>
-      </c>
-      <c r="AA39" s="17" t="s">
-        <v>397</v>
       </c>
       <c r="AB39" s="15"/>
       <c r="AC39" s="20">
@@ -12606,73 +12606,73 @@
     </row>
     <row r="40">
       <c r="A40" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>398</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>371</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>399</v>
       </c>
       <c r="D40" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="22" t="s">
+        <v>399</v>
+      </c>
+      <c r="G40" s="22" t="s">
         <v>400</v>
-      </c>
-      <c r="G40" s="22" t="s">
-        <v>401</v>
       </c>
       <c r="H40" s="26"/>
       <c r="I40" s="25">
         <v>1.0</v>
       </c>
       <c r="J40" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="K40" s="22" t="s">
         <v>402</v>
-      </c>
-      <c r="K40" s="22" t="s">
-        <v>403</v>
       </c>
       <c r="L40" s="26"/>
       <c r="M40" s="25">
         <v>1.0</v>
       </c>
       <c r="N40" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="O40" s="22" t="s">
         <v>404</v>
-      </c>
-      <c r="O40" s="22" t="s">
-        <v>405</v>
       </c>
       <c r="P40" s="26"/>
       <c r="Q40" s="25">
         <v>1.0</v>
       </c>
       <c r="R40" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="S40" s="22" t="s">
         <v>406</v>
-      </c>
-      <c r="S40" s="22" t="s">
-        <v>407</v>
       </c>
       <c r="T40" s="26"/>
       <c r="U40" s="25">
         <v>1.0</v>
       </c>
       <c r="V40" s="22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="W40" s="22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="X40" s="26"/>
       <c r="Y40" s="25">
         <v>1.0</v>
       </c>
       <c r="Z40" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="AA40" s="22" t="s">
         <v>409</v>
-      </c>
-      <c r="AA40" s="22" t="s">
-        <v>410</v>
       </c>
       <c r="AB40" s="26"/>
       <c r="AC40" s="27">
@@ -12685,7 +12685,7 @@
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D41" s="28" t="s">
         <v>37</v>
@@ -12694,20 +12694,20 @@
         <v>38</v>
       </c>
       <c r="F41" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="G41" s="17" t="s">
         <v>412</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>413</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="19">
         <v>1.0</v>
       </c>
       <c r="J41" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="K41" s="17" t="s">
         <v>414</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>415</v>
       </c>
       <c r="L41" s="34">
         <v>44340.0</v>
@@ -12716,40 +12716,40 @@
         <v>1.0</v>
       </c>
       <c r="N41" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="O41" s="17" t="s">
         <v>416</v>
-      </c>
-      <c r="O41" s="17" t="s">
-        <v>417</v>
       </c>
       <c r="P41" s="15"/>
       <c r="Q41" s="19">
         <v>1.0</v>
       </c>
       <c r="R41" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="S41" s="17" t="s">
         <v>418</v>
-      </c>
-      <c r="S41" s="17" t="s">
-        <v>419</v>
       </c>
       <c r="T41" s="15"/>
       <c r="U41" s="19">
         <v>1.0</v>
       </c>
       <c r="V41" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="W41" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="X41" s="15"/>
       <c r="Y41" s="19">
         <v>1.0</v>
       </c>
       <c r="Z41" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AA41" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AB41" s="15"/>
       <c r="AC41" s="20">
@@ -12758,73 +12758,73 @@
     </row>
     <row r="42">
       <c r="A42" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B42" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>371</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>372</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="G42" s="22" t="s">
         <v>422</v>
-      </c>
-      <c r="G42" s="22" t="s">
-        <v>423</v>
       </c>
       <c r="H42" s="26"/>
       <c r="I42" s="25">
         <v>1.0</v>
       </c>
       <c r="J42" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="K42" s="22" t="s">
         <v>424</v>
-      </c>
-      <c r="K42" s="22" t="s">
-        <v>425</v>
       </c>
       <c r="L42" s="26"/>
       <c r="M42" s="25">
         <v>1.0</v>
       </c>
       <c r="N42" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="O42" s="22" t="s">
         <v>426</v>
-      </c>
-      <c r="O42" s="22" t="s">
-        <v>427</v>
       </c>
       <c r="P42" s="26"/>
       <c r="Q42" s="25">
         <v>1.0</v>
       </c>
       <c r="R42" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S42" s="22" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="T42" s="26"/>
       <c r="U42" s="25">
         <v>1.0</v>
       </c>
       <c r="V42" s="22" t="s">
+        <v>428</v>
+      </c>
+      <c r="W42" s="22" t="s">
         <v>429</v>
-      </c>
-      <c r="W42" s="22" t="s">
-        <v>430</v>
       </c>
       <c r="X42" s="26"/>
       <c r="Y42" s="25">
         <v>1.0</v>
       </c>
       <c r="Z42" s="22" t="s">
+        <v>430</v>
+      </c>
+      <c r="AA42" s="22" t="s">
         <v>431</v>
-      </c>
-      <c r="AA42" s="22" t="s">
-        <v>432</v>
       </c>
       <c r="AB42" s="26"/>
       <c r="AC42" s="27">
@@ -12833,23 +12833,23 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>434</v>
-      </c>
       <c r="C43" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H43" s="15"/>
       <c r="I43" s="19">
@@ -12859,7 +12859,7 @@
         <v>36</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="L43" s="15"/>
       <c r="M43" s="19">
@@ -12869,17 +12869,17 @@
         <v>40</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="P43" s="15"/>
       <c r="Q43" s="19">
         <v>1.0</v>
       </c>
       <c r="R43" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S43" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="T43" s="15"/>
       <c r="U43" s="19">
@@ -12889,17 +12889,17 @@
         <v>40</v>
       </c>
       <c r="W43" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="X43" s="15"/>
       <c r="Y43" s="19">
         <v>1.0</v>
       </c>
       <c r="Z43" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA43" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AB43" s="15"/>
       <c r="AC43" s="20">
@@ -12908,73 +12908,73 @@
     </row>
     <row r="44">
       <c r="A44" s="21" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E44" s="26"/>
       <c r="F44" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="G44" s="22" t="s">
         <v>442</v>
-      </c>
-      <c r="G44" s="22" t="s">
-        <v>443</v>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="25">
         <v>1.0</v>
       </c>
       <c r="J44" s="22" t="s">
+        <v>443</v>
+      </c>
+      <c r="K44" s="22" t="s">
         <v>444</v>
-      </c>
-      <c r="K44" s="22" t="s">
-        <v>445</v>
       </c>
       <c r="L44" s="26"/>
       <c r="M44" s="25">
         <v>1.0</v>
       </c>
       <c r="N44" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="O44" s="22" t="s">
         <v>446</v>
-      </c>
-      <c r="O44" s="22" t="s">
-        <v>447</v>
       </c>
       <c r="P44" s="26"/>
       <c r="Q44" s="25">
         <v>1.0</v>
       </c>
       <c r="R44" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="S44" s="22" t="s">
         <v>448</v>
-      </c>
-      <c r="S44" s="22" t="s">
-        <v>449</v>
       </c>
       <c r="T44" s="26"/>
       <c r="U44" s="25">
         <v>1.0</v>
       </c>
       <c r="V44" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="W44" s="22" t="s">
         <v>450</v>
-      </c>
-      <c r="W44" s="22" t="s">
-        <v>451</v>
       </c>
       <c r="X44" s="26"/>
       <c r="Y44" s="25">
         <v>1.0</v>
       </c>
       <c r="Z44" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="AA44" s="22" t="s">
         <v>452</v>
-      </c>
-      <c r="AA44" s="22" t="s">
-        <v>453</v>
       </c>
       <c r="AB44" s="26"/>
       <c r="AC44" s="27">
@@ -12983,73 +12983,73 @@
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D45" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="17" t="s">
+        <v>454</v>
+      </c>
+      <c r="G45" s="17" t="s">
         <v>455</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>456</v>
       </c>
       <c r="H45" s="15"/>
       <c r="I45" s="19">
         <v>1.0</v>
       </c>
       <c r="J45" s="17" t="s">
+        <v>456</v>
+      </c>
+      <c r="K45" s="17" t="s">
         <v>457</v>
-      </c>
-      <c r="K45" s="17" t="s">
-        <v>458</v>
       </c>
       <c r="L45" s="15"/>
       <c r="M45" s="19">
         <v>1.0</v>
       </c>
       <c r="N45" s="17" t="s">
+        <v>458</v>
+      </c>
+      <c r="O45" s="17" t="s">
         <v>459</v>
-      </c>
-      <c r="O45" s="17" t="s">
-        <v>460</v>
       </c>
       <c r="P45" s="15"/>
       <c r="Q45" s="19">
         <v>1.0</v>
       </c>
       <c r="R45" s="17" t="s">
+        <v>460</v>
+      </c>
+      <c r="S45" s="17" t="s">
         <v>461</v>
-      </c>
-      <c r="S45" s="17" t="s">
-        <v>462</v>
       </c>
       <c r="T45" s="15"/>
       <c r="U45" s="19">
         <v>1.0</v>
       </c>
       <c r="V45" s="17" t="s">
+        <v>462</v>
+      </c>
+      <c r="W45" s="17" t="s">
         <v>463</v>
-      </c>
-      <c r="W45" s="17" t="s">
-        <v>464</v>
       </c>
       <c r="X45" s="15"/>
       <c r="Y45" s="19">
         <v>1.0</v>
       </c>
       <c r="Z45" s="17" t="s">
+        <v>464</v>
+      </c>
+      <c r="AA45" s="17" t="s">
         <v>465</v>
-      </c>
-      <c r="AA45" s="17" t="s">
-        <v>466</v>
       </c>
       <c r="AB45" s="15"/>
       <c r="AC45" s="20">
@@ -13058,73 +13058,73 @@
     </row>
     <row r="46">
       <c r="A46" s="21" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="G46" s="22" t="s">
         <v>468</v>
-      </c>
-      <c r="G46" s="22" t="s">
-        <v>469</v>
       </c>
       <c r="H46" s="26"/>
       <c r="I46" s="25">
         <v>1.0</v>
       </c>
       <c r="J46" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="K46" s="22" t="s">
         <v>470</v>
-      </c>
-      <c r="K46" s="22" t="s">
-        <v>471</v>
       </c>
       <c r="L46" s="26"/>
       <c r="M46" s="25">
         <v>1.0</v>
       </c>
       <c r="N46" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="O46" s="22" t="s">
         <v>472</v>
-      </c>
-      <c r="O46" s="22" t="s">
-        <v>473</v>
       </c>
       <c r="P46" s="26"/>
       <c r="Q46" s="25">
         <v>1.0</v>
       </c>
       <c r="R46" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="S46" s="22" t="s">
         <v>474</v>
-      </c>
-      <c r="S46" s="22" t="s">
-        <v>475</v>
       </c>
       <c r="T46" s="26"/>
       <c r="U46" s="25">
         <v>1.0</v>
       </c>
       <c r="V46" s="22" t="s">
+        <v>475</v>
+      </c>
+      <c r="W46" s="22" t="s">
         <v>476</v>
-      </c>
-      <c r="W46" s="22" t="s">
-        <v>477</v>
       </c>
       <c r="X46" s="26"/>
       <c r="Y46" s="25">
         <v>1.0</v>
       </c>
       <c r="Z46" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA46" s="22" t="s">
         <v>478</v>
-      </c>
-      <c r="AA46" s="22" t="s">
-        <v>479</v>
       </c>
       <c r="AB46" s="26"/>
       <c r="AC46" s="27">
@@ -13133,73 +13133,73 @@
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D47" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="G47" s="17" t="s">
         <v>481</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>482</v>
       </c>
       <c r="H47" s="15"/>
       <c r="I47" s="19">
         <v>1.0</v>
       </c>
       <c r="J47" s="17" t="s">
+        <v>482</v>
+      </c>
+      <c r="K47" s="17" t="s">
         <v>483</v>
-      </c>
-      <c r="K47" s="17" t="s">
-        <v>484</v>
       </c>
       <c r="L47" s="15"/>
       <c r="M47" s="19">
         <v>1.0</v>
       </c>
       <c r="N47" s="17" t="s">
+        <v>484</v>
+      </c>
+      <c r="O47" s="17" t="s">
         <v>485</v>
-      </c>
-      <c r="O47" s="17" t="s">
-        <v>486</v>
       </c>
       <c r="P47" s="15"/>
       <c r="Q47" s="19">
         <v>1.0</v>
       </c>
       <c r="R47" s="17" t="s">
+        <v>486</v>
+      </c>
+      <c r="S47" s="17" t="s">
         <v>487</v>
-      </c>
-      <c r="S47" s="17" t="s">
-        <v>488</v>
       </c>
       <c r="T47" s="15"/>
       <c r="U47" s="19">
         <v>1.0</v>
       </c>
       <c r="V47" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="W47" s="17" t="s">
         <v>489</v>
-      </c>
-      <c r="W47" s="17" t="s">
-        <v>490</v>
       </c>
       <c r="X47" s="15"/>
       <c r="Y47" s="19">
         <v>1.0</v>
       </c>
       <c r="Z47" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="AA47" s="17" t="s">
         <v>491</v>
-      </c>
-      <c r="AA47" s="17" t="s">
-        <v>492</v>
       </c>
       <c r="AB47" s="15"/>
       <c r="AC47" s="20">
@@ -13208,73 +13208,73 @@
     </row>
     <row r="48">
       <c r="A48" s="21" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="G48" s="22" t="s">
         <v>494</v>
-      </c>
-      <c r="G48" s="22" t="s">
-        <v>495</v>
       </c>
       <c r="H48" s="26"/>
       <c r="I48" s="25">
         <v>1.0</v>
       </c>
       <c r="J48" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="K48" s="22" t="s">
         <v>496</v>
-      </c>
-      <c r="K48" s="22" t="s">
-        <v>497</v>
       </c>
       <c r="L48" s="26"/>
       <c r="M48" s="25">
         <v>1.0</v>
       </c>
       <c r="N48" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="O48" s="22" t="s">
         <v>498</v>
-      </c>
-      <c r="O48" s="22" t="s">
-        <v>499</v>
       </c>
       <c r="P48" s="26"/>
       <c r="Q48" s="25">
         <v>1.0</v>
       </c>
       <c r="R48" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="S48" s="22" t="s">
         <v>500</v>
-      </c>
-      <c r="S48" s="22" t="s">
-        <v>501</v>
       </c>
       <c r="T48" s="26"/>
       <c r="U48" s="25">
         <v>1.0</v>
       </c>
       <c r="V48" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="W48" s="22" t="s">
         <v>502</v>
-      </c>
-      <c r="W48" s="22" t="s">
-        <v>503</v>
       </c>
       <c r="X48" s="26"/>
       <c r="Y48" s="25">
         <v>1.0</v>
       </c>
       <c r="Z48" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="AA48" s="22" t="s">
         <v>504</v>
-      </c>
-      <c r="AA48" s="22" t="s">
-        <v>505</v>
       </c>
       <c r="AB48" s="26"/>
       <c r="AC48" s="27">
@@ -13283,73 +13283,73 @@
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="C49" s="17" t="s">
         <v>506</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>434</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>507</v>
       </c>
       <c r="D49" s="28" t="s">
         <v>37</v>
       </c>
       <c r="E49" s="15"/>
       <c r="F49" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="G49" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>509</v>
       </c>
       <c r="H49" s="15"/>
       <c r="I49" s="19">
         <v>1.0</v>
       </c>
       <c r="J49" s="17" t="s">
+        <v>509</v>
+      </c>
+      <c r="K49" s="17" t="s">
         <v>510</v>
-      </c>
-      <c r="K49" s="17" t="s">
-        <v>511</v>
       </c>
       <c r="L49" s="15"/>
       <c r="M49" s="19">
         <v>1.0</v>
       </c>
       <c r="N49" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="O49" s="17" t="s">
         <v>512</v>
-      </c>
-      <c r="O49" s="17" t="s">
-        <v>513</v>
       </c>
       <c r="P49" s="15"/>
       <c r="Q49" s="19">
         <v>1.0</v>
       </c>
       <c r="R49" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="S49" s="17" t="s">
         <v>514</v>
-      </c>
-      <c r="S49" s="17" t="s">
-        <v>515</v>
       </c>
       <c r="T49" s="15"/>
       <c r="U49" s="19">
         <v>1.0</v>
       </c>
       <c r="V49" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="W49" s="17" t="s">
         <v>516</v>
-      </c>
-      <c r="W49" s="17" t="s">
-        <v>517</v>
       </c>
       <c r="X49" s="15"/>
       <c r="Y49" s="19">
         <v>1.0</v>
       </c>
       <c r="Z49" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="AA49" s="17" t="s">
         <v>518</v>
-      </c>
-      <c r="AA49" s="17" t="s">
-        <v>519</v>
       </c>
       <c r="AB49" s="15"/>
       <c r="AC49" s="20">
@@ -13358,73 +13358,73 @@
     </row>
     <row r="50">
       <c r="A50" s="21" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D50" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E50" s="26"/>
       <c r="F50" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="G50" s="22" t="s">
         <v>521</v>
-      </c>
-      <c r="G50" s="22" t="s">
-        <v>522</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="25">
         <v>1.0</v>
       </c>
       <c r="J50" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="K50" s="22" t="s">
         <v>523</v>
-      </c>
-      <c r="K50" s="22" t="s">
-        <v>524</v>
       </c>
       <c r="L50" s="26"/>
       <c r="M50" s="25">
         <v>1.0</v>
       </c>
       <c r="N50" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="O50" s="22" t="s">
         <v>525</v>
-      </c>
-      <c r="O50" s="22" t="s">
-        <v>526</v>
       </c>
       <c r="P50" s="26"/>
       <c r="Q50" s="25">
         <v>1.0</v>
       </c>
       <c r="R50" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="S50" s="22" t="s">
         <v>527</v>
-      </c>
-      <c r="S50" s="22" t="s">
-        <v>528</v>
       </c>
       <c r="T50" s="26"/>
       <c r="U50" s="25">
         <v>1.0</v>
       </c>
       <c r="V50" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="W50" s="22" t="s">
         <v>529</v>
-      </c>
-      <c r="W50" s="22" t="s">
-        <v>530</v>
       </c>
       <c r="X50" s="26"/>
       <c r="Y50" s="25">
         <v>1.0</v>
       </c>
       <c r="Z50" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="AA50" s="22" t="s">
         <v>531</v>
-      </c>
-      <c r="AA50" s="22" t="s">
-        <v>532</v>
       </c>
       <c r="AB50" s="26"/>
       <c r="AC50" s="27">
@@ -13436,16 +13436,16 @@
         <v>36</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="30"/>
       <c r="E51" s="15"/>
       <c r="F51" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H51" s="15"/>
       <c r="I51" s="19">
@@ -13455,7 +13455,7 @@
         <v>36</v>
       </c>
       <c r="K51" s="17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L51" s="15"/>
       <c r="M51" s="19">
@@ -13465,17 +13465,17 @@
         <v>40</v>
       </c>
       <c r="O51" s="17" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="P51" s="15"/>
       <c r="Q51" s="19">
         <v>1.0</v>
       </c>
       <c r="R51" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S51" s="17" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="T51" s="15"/>
       <c r="U51" s="19">
@@ -13485,17 +13485,17 @@
         <v>40</v>
       </c>
       <c r="W51" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X51" s="15"/>
       <c r="Y51" s="19">
         <v>1.0</v>
       </c>
       <c r="Z51" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA51" s="17" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AB51" s="15"/>
       <c r="AC51" s="20">
@@ -13504,10 +13504,10 @@
     </row>
     <row r="52">
       <c r="A52" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="B52" s="22" t="s">
         <v>540</v>
-      </c>
-      <c r="B52" s="22" t="s">
-        <v>541</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>92</v>
@@ -13517,62 +13517,62 @@
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="22" t="s">
+        <v>541</v>
+      </c>
+      <c r="G52" s="22" t="s">
         <v>542</v>
-      </c>
-      <c r="G52" s="22" t="s">
-        <v>543</v>
       </c>
       <c r="H52" s="26"/>
       <c r="I52" s="25">
         <v>1.0</v>
       </c>
       <c r="J52" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="K52" s="22" t="s">
         <v>544</v>
       </c>
-      <c r="K52" s="22" t="s">
+      <c r="L52" s="22" t="s">
         <v>545</v>
       </c>
-      <c r="L52" s="22" t="s">
+      <c r="M52" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="N52" s="22" t="s">
         <v>546</v>
       </c>
-      <c r="M52" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="N52" s="22" t="s">
+      <c r="O52" s="22" t="s">
         <v>547</v>
-      </c>
-      <c r="O52" s="22" t="s">
-        <v>548</v>
       </c>
       <c r="P52" s="26"/>
       <c r="Q52" s="25">
         <v>1.0</v>
       </c>
       <c r="R52" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="S52" s="22" t="s">
         <v>549</v>
-      </c>
-      <c r="S52" s="22" t="s">
-        <v>550</v>
       </c>
       <c r="T52" s="26"/>
       <c r="U52" s="25">
         <v>1.0</v>
       </c>
       <c r="V52" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="W52" s="22" t="s">
         <v>551</v>
-      </c>
-      <c r="W52" s="22" t="s">
-        <v>552</v>
       </c>
       <c r="X52" s="26"/>
       <c r="Y52" s="25">
         <v>1.0</v>
       </c>
       <c r="Z52" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="AA52" s="22" t="s">
         <v>553</v>
-      </c>
-      <c r="AA52" s="22" t="s">
-        <v>554</v>
       </c>
       <c r="AB52" s="26"/>
       <c r="AC52" s="27">
@@ -13581,10 +13581,10 @@
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>555</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>556</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>92</v>
@@ -13594,62 +13594,62 @@
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="17" t="s">
+        <v>556</v>
+      </c>
+      <c r="G53" s="17" t="s">
         <v>557</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>558</v>
       </c>
       <c r="H53" s="15"/>
       <c r="I53" s="19">
         <v>1.0</v>
       </c>
       <c r="J53" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="K53" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="L53" s="17" t="s">
         <v>560</v>
       </c>
-      <c r="L53" s="17" t="s">
+      <c r="M53" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="N53" s="17" t="s">
         <v>561</v>
       </c>
-      <c r="M53" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="N53" s="17" t="s">
+      <c r="O53" s="17" t="s">
         <v>562</v>
-      </c>
-      <c r="O53" s="17" t="s">
-        <v>563</v>
       </c>
       <c r="P53" s="15"/>
       <c r="Q53" s="19">
         <v>1.0</v>
       </c>
       <c r="R53" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="S53" s="17" t="s">
         <v>564</v>
-      </c>
-      <c r="S53" s="17" t="s">
-        <v>565</v>
       </c>
       <c r="T53" s="15"/>
       <c r="U53" s="19">
         <v>1.0</v>
       </c>
       <c r="V53" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="W53" s="17" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="X53" s="15"/>
       <c r="Y53" s="19">
         <v>1.0</v>
       </c>
       <c r="Z53" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="AA53" s="17" t="s">
         <v>567</v>
-      </c>
-      <c r="AA53" s="17" t="s">
-        <v>568</v>
       </c>
       <c r="AB53" s="15"/>
       <c r="AC53" s="20">
@@ -13658,10 +13658,10 @@
     </row>
     <row r="54">
       <c r="A54" s="21" t="s">
+        <v>568</v>
+      </c>
+      <c r="B54" s="22" t="s">
         <v>569</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>570</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>44</v>
@@ -13671,20 +13671,20 @@
       </c>
       <c r="E54" s="26"/>
       <c r="F54" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="G54" s="22" t="s">
         <v>571</v>
-      </c>
-      <c r="G54" s="22" t="s">
-        <v>572</v>
       </c>
       <c r="H54" s="26"/>
       <c r="I54" s="25">
         <v>1.0</v>
       </c>
       <c r="J54" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="K54" s="22" t="s">
         <v>573</v>
-      </c>
-      <c r="K54" s="22" t="s">
-        <v>574</v>
       </c>
       <c r="L54" s="35">
         <v>21045.0</v>
@@ -13696,37 +13696,37 @@
         <v>48</v>
       </c>
       <c r="O54" s="22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="P54" s="26"/>
       <c r="Q54" s="25">
         <v>1.0</v>
       </c>
       <c r="R54" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="S54" s="22" t="s">
         <v>576</v>
-      </c>
-      <c r="S54" s="22" t="s">
-        <v>577</v>
       </c>
       <c r="T54" s="26"/>
       <c r="U54" s="25">
         <v>1.0</v>
       </c>
       <c r="V54" s="22" t="s">
+        <v>577</v>
+      </c>
+      <c r="W54" s="22" t="s">
         <v>578</v>
-      </c>
-      <c r="W54" s="22" t="s">
-        <v>579</v>
       </c>
       <c r="X54" s="26"/>
       <c r="Y54" s="25">
         <v>1.0</v>
       </c>
       <c r="Z54" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="AA54" s="22" t="s">
         <v>580</v>
-      </c>
-      <c r="AA54" s="22" t="s">
-        <v>581</v>
       </c>
       <c r="AB54" s="26"/>
       <c r="AC54" s="27">
@@ -13735,10 +13735,10 @@
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>582</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>583</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>92</v>
@@ -13748,23 +13748,23 @@
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="17" t="s">
+        <v>583</v>
+      </c>
+      <c r="G55" s="17" t="s">
         <v>584</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>585</v>
       </c>
       <c r="H55" s="15"/>
       <c r="I55" s="19">
         <v>1.0</v>
       </c>
       <c r="J55" s="17" t="s">
+        <v>585</v>
+      </c>
+      <c r="K55" s="17" t="s">
         <v>586</v>
       </c>
-      <c r="K55" s="17" t="s">
+      <c r="L55" s="17" t="s">
         <v>587</v>
-      </c>
-      <c r="L55" s="17" t="s">
-        <v>588</v>
       </c>
       <c r="M55" s="19">
         <v>1.0</v>
@@ -13773,37 +13773,37 @@
         <v>54</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="P55" s="15"/>
       <c r="Q55" s="19">
         <v>1.0</v>
       </c>
       <c r="R55" s="17" t="s">
+        <v>589</v>
+      </c>
+      <c r="S55" s="17" t="s">
         <v>590</v>
-      </c>
-      <c r="S55" s="17" t="s">
-        <v>591</v>
       </c>
       <c r="T55" s="15"/>
       <c r="U55" s="19">
         <v>1.0</v>
       </c>
       <c r="V55" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="W55" s="17" t="s">
         <v>592</v>
-      </c>
-      <c r="W55" s="17" t="s">
-        <v>593</v>
       </c>
       <c r="X55" s="15"/>
       <c r="Y55" s="19">
         <v>1.0</v>
       </c>
       <c r="Z55" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="AA55" s="17" t="s">
         <v>594</v>
-      </c>
-      <c r="AA55" s="17" t="s">
-        <v>595</v>
       </c>
       <c r="AB55" s="15"/>
       <c r="AC55" s="20">
@@ -13812,75 +13812,75 @@
     </row>
     <row r="56">
       <c r="A56" s="21" t="s">
+        <v>595</v>
+      </c>
+      <c r="B56" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="B56" s="22" t="s">
-        <v>597</v>
-      </c>
       <c r="C56" s="22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D56" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E56" s="26"/>
       <c r="F56" s="22" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H56" s="26"/>
       <c r="I56" s="25">
         <v>1.0</v>
       </c>
       <c r="J56" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="K56" s="22" t="s">
         <v>599</v>
       </c>
-      <c r="K56" s="22" t="s">
+      <c r="L56" s="22" t="s">
         <v>600</v>
       </c>
-      <c r="L56" s="22" t="s">
+      <c r="M56" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="N56" s="22" t="s">
         <v>601</v>
       </c>
-      <c r="M56" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="N56" s="22" t="s">
+      <c r="O56" s="22" t="s">
         <v>602</v>
-      </c>
-      <c r="O56" s="22" t="s">
-        <v>603</v>
       </c>
       <c r="P56" s="26"/>
       <c r="Q56" s="25">
         <v>1.0</v>
       </c>
       <c r="R56" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="S56" s="22" t="s">
         <v>604</v>
-      </c>
-      <c r="S56" s="22" t="s">
-        <v>605</v>
       </c>
       <c r="T56" s="26"/>
       <c r="U56" s="25">
         <v>1.0</v>
       </c>
       <c r="V56" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="W56" s="22" t="s">
         <v>606</v>
-      </c>
-      <c r="W56" s="22" t="s">
-        <v>607</v>
       </c>
       <c r="X56" s="26"/>
       <c r="Y56" s="25">
         <v>1.0</v>
       </c>
       <c r="Z56" s="22" t="s">
+        <v>607</v>
+      </c>
+      <c r="AA56" s="22" t="s">
         <v>608</v>
-      </c>
-      <c r="AA56" s="22" t="s">
-        <v>609</v>
       </c>
       <c r="AB56" s="26"/>
       <c r="AC56" s="27">
@@ -13889,7 +13889,7 @@
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>106</v>
+        <v>609</v>
       </c>
       <c r="B57" s="36" t="s">
         <v>610</v>
@@ -34814,7 +34814,7 @@
     </row>
     <row r="400">
       <c r="A400" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B400" s="17" t="s">
         <v>2667</v>
@@ -34845,7 +34845,7 @@
         <v>1.0</v>
       </c>
       <c r="N400" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O400" s="17" t="s">
         <v>2672</v>
@@ -34865,7 +34865,7 @@
         <v>1.0</v>
       </c>
       <c r="V400" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="W400" s="17" t="s">
         <v>2675</v>
@@ -34981,7 +34981,7 @@
         <v>1.0</v>
       </c>
       <c r="J402" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K402" s="17" t="s">
         <v>2696</v>
@@ -35653,7 +35653,7 @@
     </row>
     <row r="413">
       <c r="A413" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B413" s="15"/>
       <c r="C413" s="15"/>
@@ -35668,7 +35668,7 @@
         <v>1.0</v>
       </c>
       <c r="J413" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K413" s="15"/>
       <c r="L413" s="15"/>
@@ -35723,7 +35723,7 @@
       </c>
       <c r="E414" s="26"/>
       <c r="F414" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G414" s="22" t="s">
         <v>2796</v>
@@ -35755,7 +35755,7 @@
         <v>1.0</v>
       </c>
       <c r="R414" s="22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S414" s="22" t="s">
         <v>2799</v>
@@ -35775,7 +35775,7 @@
         <v>1.0</v>
       </c>
       <c r="Z414" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA414" s="22" t="s">
         <v>2801</v>
@@ -35791,7 +35791,7 @@
       </c>
       <c r="B415" s="15"/>
       <c r="C415" s="17" t="s">
-        <v>106</v>
+        <v>609</v>
       </c>
       <c r="D415" s="33">
         <v>11.0</v>
@@ -35808,19 +35808,19 @@
         <v>1.0</v>
       </c>
       <c r="J415" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K415" s="17" t="s">
         <v>2805</v>
       </c>
       <c r="L415" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M415" s="19">
         <v>1.0</v>
       </c>
       <c r="N415" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O415" s="17" t="s">
         <v>2806</v>
@@ -35830,7 +35830,7 @@
         <v>1.0</v>
       </c>
       <c r="R415" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S415" s="17" t="s">
         <v>2807</v>
@@ -35840,7 +35840,7 @@
         <v>1.0</v>
       </c>
       <c r="V415" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="W415" s="17" t="s">
         <v>2808</v>
@@ -35850,7 +35850,7 @@
         <v>1.0</v>
       </c>
       <c r="Z415" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AA415" s="17" t="s">
         <v>2809</v>
@@ -36633,7 +36633,7 @@
         <v>1.0</v>
       </c>
       <c r="R426" s="22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S426" s="22" t="s">
         <v>2942</v>
@@ -36653,7 +36653,7 @@
         <v>1.0</v>
       </c>
       <c r="Z426" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA426" s="22" t="s">
         <v>2944</v>
@@ -36712,7 +36712,7 @@
         <v>1.0</v>
       </c>
       <c r="R427" s="17" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="S427" s="17" t="s">
         <v>2950</v>
@@ -36722,7 +36722,7 @@
         <v>1.0</v>
       </c>
       <c r="V427" s="17" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="W427" s="17" t="s">
         <v>2951</v>
@@ -36732,7 +36732,7 @@
         <v>1.0</v>
       </c>
       <c r="Z427" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AA427" s="17" t="s">
         <v>2952</v>
@@ -36755,7 +36755,7 @@
       </c>
       <c r="E428" s="26"/>
       <c r="F428" s="22" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G428" s="22" t="s">
         <v>2954</v>
@@ -36785,7 +36785,7 @@
         <v>1.0</v>
       </c>
       <c r="R428" s="22" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="S428" s="22" t="s">
         <v>2957</v>
@@ -36795,7 +36795,7 @@
         <v>1.0</v>
       </c>
       <c r="V428" s="22" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="W428" s="22" t="s">
         <v>2958</v>
@@ -36805,7 +36805,7 @@
         <v>1.0</v>
       </c>
       <c r="Z428" s="22" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AA428" s="22" t="s">
         <v>2959</v>
@@ -37142,7 +37142,7 @@
         <v>3000</v>
       </c>
       <c r="C434" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D434" s="29">
         <v>10.0</v>
@@ -37191,7 +37191,7 @@
       </c>
       <c r="B435" s="15"/>
       <c r="C435" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D435" s="33">
         <v>10.0</v>
@@ -37302,7 +37302,7 @@
         <v>74</v>
       </c>
       <c r="D437" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E437" s="15"/>
       <c r="F437" s="17" t="s">
@@ -37482,7 +37482,7 @@
         <v>1.0</v>
       </c>
       <c r="R439" s="22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S439" s="22" t="s">
         <v>3037</v>
@@ -37502,7 +37502,7 @@
         <v>1.0</v>
       </c>
       <c r="Z439" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA439" s="22" t="s">
         <v>3039</v>
@@ -37565,7 +37565,7 @@
         <v>1.0</v>
       </c>
       <c r="R440" s="17" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="S440" s="17" t="s">
         <v>3045</v>
@@ -37575,7 +37575,7 @@
         <v>1.0</v>
       </c>
       <c r="V440" s="17" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="W440" s="17" t="s">
         <v>3046</v>
@@ -37585,7 +37585,7 @@
         <v>1.0</v>
       </c>
       <c r="Z440" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AA440" s="17" t="s">
         <v>3047</v>
@@ -37608,7 +37608,7 @@
       </c>
       <c r="E441" s="26"/>
       <c r="F441" s="22" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G441" s="22" t="s">
         <v>3049</v>
@@ -37638,7 +37638,7 @@
         <v>1.0</v>
       </c>
       <c r="R441" s="22" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="S441" s="22" t="s">
         <v>3052</v>
@@ -37648,7 +37648,7 @@
         <v>1.0</v>
       </c>
       <c r="V441" s="22" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="W441" s="22" t="s">
         <v>3053</v>
@@ -37658,7 +37658,7 @@
         <v>1.0</v>
       </c>
       <c r="Z441" s="22" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AA441" s="22" t="s">
         <v>3054</v>
@@ -38133,7 +38133,7 @@
       </c>
       <c r="B449" s="26"/>
       <c r="C449" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D449" s="29">
         <v>10.0</v>
@@ -38191,13 +38191,13 @@
         <v>3115</v>
       </c>
       <c r="B450" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C450" s="17" t="s">
         <v>92</v>
       </c>
       <c r="D450" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E450" s="15"/>
       <c r="F450" s="17" t="s">
@@ -38272,13 +38272,13 @@
         <v>3130</v>
       </c>
       <c r="B451" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C451" s="22" t="s">
         <v>92</v>
       </c>
       <c r="D451" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E451" s="26"/>
       <c r="F451" s="22" t="s">
@@ -38578,7 +38578,7 @@
         <v>3184</v>
       </c>
       <c r="B455" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C455" s="22" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
GUI terms translation review
Using google sheet function googletranslate
</commit_message>
<xml_diff>
--- a/material/translation/DomicileRegistrationEvidence/MOR2_ro_en_es_sl_pt_fr.xlsx
+++ b/material/translation/DomicileRegistrationEvidence/MOR2_ro_en_es_sl_pt_fr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4736" uniqueCount="3348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4679" uniqueCount="3294">
   <si>
     <t>Term URI</t>
   </si>
@@ -9743,9 +9743,6 @@
     <t>xs:string</t>
   </si>
   <si>
-    <t>Dovezi Canonice</t>
-  </si>
-  <si>
     <t>Dovada emisă de autoritatea competentă în forma canonică a acelui tip de probe</t>
   </si>
   <si>
@@ -9761,30 +9758,12 @@
     <t>Evidencia emitida por la autoridad competente en la forma canónica de ese tipo de evidence</t>
   </si>
   <si>
-    <t>Kanonični dokazi</t>
-  </si>
-  <si>
     <t>Dokazilo, ki ga izda pristojni organ v kanonični obliki te vrste dokazila</t>
   </si>
   <si>
-    <t>Evidência Canônica</t>
-  </si>
-  <si>
-    <t>Provas emitidas pela autoridade competente na forma canónica desse tipo de prova</t>
-  </si>
-  <si>
-    <t>Preuve Canonique</t>
-  </si>
-  <si>
-    <t>Preuve délivrée par l'autorité compétente sous la forme canonique de ce type de preuve</t>
-  </si>
-  <si>
     <t>GUI/DomesticEvidence</t>
   </si>
   <si>
-    <t>Dovezi domestice</t>
-  </si>
-  <si>
     <t>Dovada emisă de autoritatea competentă în forma originală în format structurat</t>
   </si>
   <si>
@@ -9800,30 +9779,12 @@
     <t>Evidencia emitida por la autoridad competente en la forma original en formato estructurado</t>
   </si>
   <si>
-    <t>Domači dokazi</t>
-  </si>
-  <si>
     <t>Dokazila, ki jih izda pristojni organ v izvirni obliki v strukturirani obliki</t>
   </si>
   <si>
-    <t>Evidência doméstica</t>
-  </si>
-  <si>
-    <t>Provas emitidas pela autoridade competente no formulário original em formato estruturado</t>
-  </si>
-  <si>
-    <t>Preuve nationale</t>
-  </si>
-  <si>
-    <t>Preuve délivrée par l'autorité compétente sous la forme originale dans un format structuré</t>
-  </si>
-  <si>
     <t>GUI/DomesticEvidencePDF</t>
   </si>
   <si>
-    <t>Dovezi interne în PDF</t>
-  </si>
-  <si>
     <t>Dovada eliberata de autoritatea competenta in format PDF</t>
   </si>
   <si>
@@ -9839,47 +9800,18 @@
     <t>Evidencia emitida por la autoridad competente en formato PDF</t>
   </si>
   <si>
-    <t>Domači dokazi v PDF</t>
-  </si>
-  <si>
     <t>Dokazila, ki jih izda pristojni organ v formatu PDF</t>
   </si>
   <si>
-    <t>Evidências domésticas em PDF</t>
-  </si>
-  <si>
-    <t>Provas emitidas pela autoridade competente em formato PDF</t>
-  </si>
-  <si>
-    <t>Preuve nationale en PDF</t>
-  </si>
-  <si>
-    <t>Preuve délivrée par l'autorité compétente au format PDF</t>
-  </si>
-  <si>
     <t>GUI/de4a-legalInfo-content/de4a-section-title</t>
   </si>
   <si>
-    <t>Informații legale</t>
-  </si>
-  <si>
     <t>Legal Info</t>
   </si>
   <si>
     <t>Información legal</t>
   </si>
   <si>
-    <t xml:space="preserve">Pravne informacije
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informação legal
-</t>
-  </si>
-  <si>
-    <t>Information légale</t>
-  </si>
-  <si>
     <t>GUI/de4a-legalInfo-content/de4a-legalInfo-yellow</t>
   </si>
   <si>
@@ -9889,26 +9821,7 @@
     <t>Lea el siguiente texto antes de continuar</t>
   </si>
   <si>
-    <t>Preden nadaljujete, preberite naslednje besedilo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leia o texto a seguir antes de continuar
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lisez le texte suivant avant de continuer
-</t>
-  </si>
-  <si>
     <t>GUI/de4a-legalInfo-content/de4a-legalInfo-text</t>
-  </si>
-  <si>
-    <t>Utilizând acest proces, ne puteți solicita direct informații relevante și vă vom furniza
-ultima versiune pe care o avem.
-Veți putea să revizuiți informațiile și să alegeți dacă să le utilizați sau nu. Nu sunteți obligat să ne solicitați informații prin intermediul acestui serviciu. Dacă anulați acest proces, veți avea posibilitatea
-finalizați procesul căutând și trimițând manual informațiile.
-Vă rugăm să rețineți că acest serviciu face parte dintr-un proiect pilot. Selectând „Sunt de acord”, sunteți de acord să participați la programul pilot pe bază de voluntariat. Trebuie să utilizați informațiile pe care vi le punem la dispoziție numai în scopul de a completa
-procedura și pentru a verifica dacă procedura a fost finalizată cu succes. Consultați https://www.de4a.eu/aboutproject pentru mai multe detalii.</t>
   </si>
   <si>
     <t>By using this process, you can request relevant information directly from us, and we’ll provide you with the
@@ -9930,99 +9843,36 @@
 </t>
   </si>
   <si>
-    <t>Z uporabo tega postopka lahko neposredno od nas zahtevate ustrezne informacije in posredovali vam jih bomo
-najnovejšo različico, ki jo imamo.
-Podatke boste lahko pregledali in se odločili, ali jih želite uporabiti ali ne. Ni vam treba zahtevati informacij od nas prek te storitve. Če prekličete ta postopek, boste imeli možnost, da
-dokončajte svoj postopek z ročnim iskanjem in pošiljanjem informacij.
-Upoštevajte, da je ta storitev del pilotnega projekta. Z izbiro "Strinjam se" se strinjate s prostovoljnim sodelovanjem v pilotnem programu. Podatke, ki vam jih damo na voljo, uporabite samo za izpolnjevanje
-postopek in preveriti, ali je bil postopek uspešno zaključen. Za več podrobnosti glejte https://www.de4a.eu/aboutproject.</t>
-  </si>
-  <si>
-    <t>Ao usar este processo, você pode solicitar informações relevantes diretamente a nós e forneceremos a você o
-versão mais recente que temos.
-Você poderá revisar as informações e escolher se deseja ou não usá-las. Você não é obrigado a nos solicitar informações por meio deste serviço. Se cancelar este processo, terá a possibilidade de
-conclua seu processo pesquisando e enviando as informações manualmente.
-Observe que este serviço faz parte de um projeto piloto. Ao selecionar "Concordo", você concorda em participar do programa piloto de forma voluntária. Você só deve usar as informações que disponibilizamos para o propósito de completar o
-procedimento e para verificar se o procedimento foi concluído com sucesso. Veja https://www.de4a.eu/aboutproject para mais detalhes.</t>
-  </si>
-  <si>
-    <t>En utilisant ce processus, vous pouvez nous demander directement des informations pertinentes et nous vous fournirons les
-dernière version que nous avons.
-Vous pourrez consulter les informations et choisir de les utiliser ou non. Vous n'êtes pas obligé de nous demander des informations par le biais de ce service. Si vous annulez ce processus, vous aurez la possibilité de
-complétez votre processus en recherchant et en envoyant les informations manuellement.
-Veuillez noter que ce service fait partie d'un projet pilote. En sélectionnant "J'accepte", vous acceptez de participer au programme pilote sur une base volontaire. Vous ne devez utiliser les informations que nous mettons à votre disposition que dans le but de remplir le
-procédure et de vérifier que la procédure s'est déroulée avec succès. Voir https://www.de4a.eu/aboutproject pour plus de détails.</t>
-  </si>
-  <si>
     <t>GUI/de4a-section-header</t>
   </si>
   <si>
-    <t>Dovezi furnizate de</t>
-  </si>
-  <si>
     <t>Evidence provided by</t>
   </si>
   <si>
     <t>Evidencia proporcionada por</t>
   </si>
   <si>
-    <t>Dokaze predložil</t>
-  </si>
-  <si>
-    <t>Provas fornecidas por</t>
-  </si>
-  <si>
-    <t>Preuve fournie par</t>
-  </si>
-  <si>
     <t>GUI/de4a-section-header/PID</t>
   </si>
   <si>
-    <t>Platforma de brokeraj de date a Administrației generale a statului spaniol</t>
-  </si>
-  <si>
     <t>Spanish Data Intermediation Platform of the National State Administration</t>
   </si>
   <si>
     <t>la Plataforma de Intermediación de Datos de la Administración General del Estado español</t>
   </si>
   <si>
-    <t>Platforma za posredovanje podatkov generalne uprave španske države</t>
-  </si>
-  <si>
-    <t>a Plataforma de Corretagem de Dados da Administração Geral do Estado Espanhol</t>
-  </si>
-  <si>
-    <t>la Plate-forme de courtage de données de l'administration générale de l'État espagnol</t>
-  </si>
-  <si>
     <t>GUI/de4a-section-header/issuedBy</t>
   </si>
   <si>
-    <t>emis de</t>
-  </si>
-  <si>
     <t>issued by</t>
   </si>
   <si>
     <t>emitida por</t>
   </si>
   <si>
-    <t>ki ga oddaja</t>
-  </si>
-  <si>
-    <t>emitido por</t>
-  </si>
-  <si>
-    <t>émis par</t>
-  </si>
-  <si>
     <t>GUI/de4a-section-header/INE</t>
   </si>
   <si>
-    <t>Institutului Național de Statistică (INS)</t>
-  </si>
-  <si>
     <t>National Statistical Institute (NSI)</t>
   </si>
   <si>
@@ -10032,33 +9882,15 @@
     <t>Národným inštitútom pre štatistiku (NIS)</t>
   </si>
   <si>
-    <t>Instituto Nacional de Estatística (INE)</t>
-  </si>
-  <si>
-    <t>l'Institut national de la statistique (INS)</t>
-  </si>
-  <si>
     <t>GUI/Retrieve</t>
   </si>
   <si>
-    <t>Recupera</t>
-  </si>
-  <si>
     <t>Retrieve</t>
   </si>
   <si>
     <t>Proceder</t>
   </si>
   <si>
-    <t>Pridobi</t>
-  </si>
-  <si>
-    <t>Recuperar</t>
-  </si>
-  <si>
-    <t>Récupérer</t>
-  </si>
-  <si>
     <t>GUI/Reject</t>
   </si>
   <si>
@@ -10068,31 +9900,13 @@
     <t>Rechazar</t>
   </si>
   <si>
-    <t>Zavrni</t>
-  </si>
-  <si>
-    <t>Rejeitar</t>
-  </si>
-  <si>
     <t>GUI/Requester</t>
   </si>
   <si>
-    <t>Probele solicitate vor fi transmise următoarei autorități</t>
-  </si>
-  <si>
     <t>The requested evidence shall be submitted to the following authority</t>
   </si>
   <si>
     <t>La evidencia solicitada será enviada a la siguiente autoridad</t>
-  </si>
-  <si>
-    <t>Zahtevani dokazi bodo poslani naslednjemu organu</t>
-  </si>
-  <si>
-    <t>As provas solicitadas serão enviadas à seguinte autoridade</t>
-  </si>
-  <si>
-    <t>Les preuves demandées seront envoyées à l'autorité suivante</t>
   </si>
 </sst>
 </file>
@@ -10102,7 +9916,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -10139,11 +9953,6 @@
     </font>
     <font>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -10217,7 +10026,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -10395,9 +10204,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -39516,61 +39322,67 @@
       </c>
       <c r="D457" s="58"/>
       <c r="E457" s="59"/>
-      <c r="F457" s="57" t="s">
+      <c r="F457" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N457,""es"",""ro"")"),"Dovezi canonice")</f>
+        <v>Dovezi canonice</v>
+      </c>
+      <c r="G457" s="57" t="s">
         <v>3243</v>
-      </c>
-      <c r="G457" s="57" t="s">
-        <v>3244</v>
       </c>
       <c r="H457" s="59"/>
       <c r="I457" s="57">
         <v>0.0</v>
       </c>
       <c r="J457" s="57" t="s">
+        <v>3244</v>
+      </c>
+      <c r="K457" s="57" t="s">
         <v>3245</v>
-      </c>
-      <c r="K457" s="57" t="s">
-        <v>3246</v>
       </c>
       <c r="L457" s="59"/>
       <c r="M457" s="57">
         <v>1.0</v>
       </c>
       <c r="N457" s="57" t="s">
+        <v>3246</v>
+      </c>
+      <c r="O457" s="57" t="s">
         <v>3247</v>
-      </c>
-      <c r="O457" s="57" t="s">
-        <v>3248</v>
       </c>
       <c r="P457" s="59"/>
       <c r="Q457" s="57">
         <v>1.0</v>
       </c>
-      <c r="R457" s="60" t="s">
-        <v>3249</v>
+      <c r="R457" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N457,""es"",""sl"")"),"Kanonični dokazi")</f>
+        <v>Kanonični dokazi</v>
       </c>
       <c r="S457" s="57" t="s">
-        <v>3250</v>
+        <v>3248</v>
       </c>
       <c r="T457" s="59"/>
       <c r="U457" s="57">
         <v>0.0</v>
       </c>
-      <c r="V457" s="60" t="s">
-        <v>3251</v>
-      </c>
-      <c r="W457" s="57" t="s">
-        <v>3252</v>
+      <c r="V457" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N457,""es"",""pt"")"),"Evidência canônica")</f>
+        <v>Evidência canônica</v>
+      </c>
+      <c r="W457" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(O457,""es"",""pt"")"),"Evidências emitidas pela autoridade competente na forma canônica de tais evidências")</f>
+        <v>Evidências emitidas pela autoridade competente na forma canônica de tais evidências</v>
       </c>
       <c r="X457" s="59"/>
       <c r="Y457" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z457" s="57" t="s">
-        <v>3253</v>
-      </c>
-      <c r="AA457" s="57" t="s">
-        <v>3254</v>
+      <c r="Z457" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N457,""es"",""fr"")"),"Preuves canoniques")</f>
+        <v>Preuves canoniques</v>
+      </c>
+      <c r="AA457" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(O457,""es"",""fr"")"),"Preuve émise par l'autorité compétente sous la forme canonique de ces preuves")</f>
+        <v>Preuve émise par l'autorité compétente sous la forme canonique de ces preuves</v>
       </c>
       <c r="AB457" s="59"/>
       <c r="AC457" s="57">
@@ -39579,7 +39391,7 @@
     </row>
     <row r="458">
       <c r="A458" s="57" t="s">
-        <v>3255</v>
+        <v>3249</v>
       </c>
       <c r="B458" s="57" t="s">
         <v>3242</v>
@@ -39589,61 +39401,67 @@
       </c>
       <c r="D458" s="58"/>
       <c r="E458" s="59"/>
-      <c r="F458" s="57" t="s">
-        <v>3256</v>
+      <c r="F458" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N458,""es"",""ro"")"),"Dovezi originale")</f>
+        <v>Dovezi originale</v>
       </c>
       <c r="G458" s="60" t="s">
-        <v>3257</v>
+        <v>3250</v>
       </c>
       <c r="H458" s="59"/>
       <c r="I458" s="57">
         <v>0.0</v>
       </c>
       <c r="J458" s="57" t="s">
-        <v>3258</v>
+        <v>3251</v>
       </c>
       <c r="K458" s="57" t="s">
-        <v>3259</v>
+        <v>3252</v>
       </c>
       <c r="L458" s="59"/>
       <c r="M458" s="57">
         <v>1.0</v>
       </c>
       <c r="N458" s="57" t="s">
-        <v>3260</v>
+        <v>3253</v>
       </c>
       <c r="O458" s="57" t="s">
-        <v>3261</v>
+        <v>3254</v>
       </c>
       <c r="P458" s="59"/>
       <c r="Q458" s="57">
         <v>1.0</v>
       </c>
-      <c r="R458" s="57" t="s">
-        <v>3262</v>
+      <c r="R458" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N458,""es"",""sl"")"),"Izvirni dokazi")</f>
+        <v>Izvirni dokazi</v>
       </c>
       <c r="S458" s="60" t="s">
-        <v>3263</v>
+        <v>3255</v>
       </c>
       <c r="T458" s="59"/>
       <c r="U458" s="57">
         <v>0.0</v>
       </c>
-      <c r="V458" s="57" t="s">
-        <v>3264</v>
-      </c>
-      <c r="W458" s="60" t="s">
-        <v>3265</v>
+      <c r="V458" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N458,""es"",""pt"")"),"Evidência original")</f>
+        <v>Evidência original</v>
+      </c>
+      <c r="W458" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(O458,""es"",""pt"")"),"Evidências emitidas pela autoridade competente na forma original em formato estruturado")</f>
+        <v>Evidências emitidas pela autoridade competente na forma original em formato estruturado</v>
       </c>
       <c r="X458" s="59"/>
       <c r="Y458" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z458" s="57" t="s">
-        <v>3266</v>
-      </c>
-      <c r="AA458" s="60" t="s">
-        <v>3267</v>
+      <c r="Z458" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N458,""es"",""fr"")"),"Preuves originales")</f>
+        <v>Preuves originales</v>
+      </c>
+      <c r="AA458" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(O458,""es"",""fr"")"),"Preuve émise par l'autorité compétente sous la forme originale au format structuré")</f>
+        <v>Preuve émise par l'autorité compétente sous la forme originale au format structuré</v>
       </c>
       <c r="AB458" s="59"/>
       <c r="AC458" s="57">
@@ -39652,7 +39470,7 @@
     </row>
     <row r="459">
       <c r="A459" s="57" t="s">
-        <v>3268</v>
+        <v>3256</v>
       </c>
       <c r="B459" s="57" t="s">
         <v>3242</v>
@@ -39662,61 +39480,67 @@
       </c>
       <c r="D459" s="58"/>
       <c r="E459" s="59"/>
-      <c r="F459" s="57" t="s">
-        <v>3269</v>
+      <c r="F459" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N459,""es"",""ro"")"),"Dovezi în format PDF")</f>
+        <v>Dovezi în format PDF</v>
       </c>
       <c r="G459" s="60" t="s">
-        <v>3270</v>
+        <v>3257</v>
       </c>
       <c r="H459" s="59"/>
       <c r="I459" s="57">
         <v>0.0</v>
       </c>
       <c r="J459" s="57" t="s">
-        <v>3271</v>
+        <v>3258</v>
       </c>
       <c r="K459" s="57" t="s">
-        <v>3272</v>
+        <v>3259</v>
       </c>
       <c r="L459" s="59"/>
       <c r="M459" s="57">
         <v>1.0</v>
       </c>
       <c r="N459" s="57" t="s">
-        <v>3273</v>
+        <v>3260</v>
       </c>
       <c r="O459" s="57" t="s">
-        <v>3274</v>
+        <v>3261</v>
       </c>
       <c r="P459" s="59"/>
       <c r="Q459" s="57">
         <v>1.0</v>
       </c>
-      <c r="R459" s="57" t="s">
-        <v>3275</v>
+      <c r="R459" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N459,""es"",""sl"")"),"Dokazi v obliki pdf")</f>
+        <v>Dokazi v obliki pdf</v>
       </c>
       <c r="S459" s="60" t="s">
-        <v>3276</v>
+        <v>3262</v>
       </c>
       <c r="T459" s="59"/>
       <c r="U459" s="57">
         <v>0.0</v>
       </c>
-      <c r="V459" s="57" t="s">
-        <v>3277</v>
-      </c>
-      <c r="W459" s="60" t="s">
-        <v>3278</v>
+      <c r="V459" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N459,""es"",""pt"")"),"Evidência em formato PDF")</f>
+        <v>Evidência em formato PDF</v>
+      </c>
+      <c r="W459" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(O459,""es"",""pt"")"),"Evidências emitidas pela autoridade competente em formato PDF")</f>
+        <v>Evidências emitidas pela autoridade competente em formato PDF</v>
       </c>
       <c r="X459" s="59"/>
       <c r="Y459" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z459" s="57" t="s">
-        <v>3279</v>
-      </c>
-      <c r="AA459" s="60" t="s">
-        <v>3280</v>
+      <c r="Z459" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N459,""es"",""fr"")"),"Preuve au format PDF")</f>
+        <v>Preuve au format PDF</v>
+      </c>
+      <c r="AA459" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(O459,""es"",""fr"")"),"Preuve émise par l'autorité compétente au format PDF")</f>
+        <v>Preuve émise par l'autorité compétente au format PDF</v>
       </c>
       <c r="AB459" s="59"/>
       <c r="AC459" s="57">
@@ -39725,7 +39549,7 @@
     </row>
     <row r="460">
       <c r="A460" s="57" t="s">
-        <v>3281</v>
+        <v>3263</v>
       </c>
       <c r="B460" s="57" t="s">
         <v>3242</v>
@@ -39735,8 +39559,9 @@
       </c>
       <c r="D460" s="58"/>
       <c r="E460" s="59"/>
-      <c r="F460" s="57" t="s">
-        <v>3282</v>
+      <c r="F460" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N460,""es"",""ro"")"),"Informații legale")</f>
+        <v>Informații legale</v>
       </c>
       <c r="G460" s="59"/>
       <c r="H460" s="59"/>
@@ -39744,7 +39569,7 @@
         <v>0.0</v>
       </c>
       <c r="J460" s="60" t="s">
-        <v>3283</v>
+        <v>3264</v>
       </c>
       <c r="K460" s="59"/>
       <c r="L460" s="59"/>
@@ -39752,31 +39577,34 @@
         <v>1.0</v>
       </c>
       <c r="N460" s="60" t="s">
-        <v>3284</v>
+        <v>3265</v>
       </c>
       <c r="O460" s="59"/>
       <c r="P460" s="59"/>
       <c r="Q460" s="57">
         <v>1.0</v>
       </c>
-      <c r="R460" s="57" t="s">
-        <v>3285</v>
+      <c r="R460" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N460,""es"",""sl"")"),"Pravne informacije")</f>
+        <v>Pravne informacije</v>
       </c>
       <c r="S460" s="59"/>
       <c r="T460" s="59"/>
       <c r="U460" s="57">
         <v>0.0</v>
       </c>
-      <c r="V460" s="57" t="s">
-        <v>3286</v>
+      <c r="V460" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N460,""es"",""pt"")"),"Informação legal")</f>
+        <v>Informação legal</v>
       </c>
       <c r="W460" s="59"/>
       <c r="X460" s="59"/>
       <c r="Y460" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z460" s="57" t="s">
-        <v>3287</v>
+      <c r="Z460" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N460,""es"",""fr"")"),"Information légale")</f>
+        <v>Information légale</v>
       </c>
       <c r="AA460" s="59"/>
       <c r="AB460" s="59"/>
@@ -39786,7 +39614,7 @@
     </row>
     <row r="461">
       <c r="A461" s="57" t="s">
-        <v>3288</v>
+        <v>3266</v>
       </c>
       <c r="B461" s="57" t="s">
         <v>3242</v>
@@ -39796,8 +39624,9 @@
       </c>
       <c r="D461" s="58"/>
       <c r="E461" s="59"/>
-      <c r="F461" s="57" t="s">
-        <v>3282</v>
+      <c r="F461" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N461,""es"",""ro"")"),"Citiți următorul text înainte de a continua")</f>
+        <v>Citiți următorul text înainte de a continua</v>
       </c>
       <c r="G461" s="59"/>
       <c r="H461" s="59"/>
@@ -39805,7 +39634,7 @@
         <v>0.0</v>
       </c>
       <c r="J461" s="60" t="s">
-        <v>3289</v>
+        <v>3267</v>
       </c>
       <c r="K461" s="59"/>
       <c r="L461" s="59"/>
@@ -39813,31 +39642,34 @@
         <v>1.0</v>
       </c>
       <c r="N461" s="60" t="s">
-        <v>3290</v>
+        <v>3268</v>
       </c>
       <c r="O461" s="59"/>
       <c r="P461" s="59"/>
       <c r="Q461" s="57">
         <v>1.0</v>
       </c>
-      <c r="R461" s="57" t="s">
-        <v>3291</v>
+      <c r="R461" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N461,""es"",""sl"")"),"Pred nadaljevanjem preberite naslednje besedilo")</f>
+        <v>Pred nadaljevanjem preberite naslednje besedilo</v>
       </c>
       <c r="S461" s="59"/>
       <c r="T461" s="59"/>
       <c r="U461" s="57">
         <v>0.0</v>
       </c>
-      <c r="V461" s="57" t="s">
-        <v>3292</v>
+      <c r="V461" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N461,""es"",""pt"")"),"Leia o seguinte texto antes de continuar")</f>
+        <v>Leia o seguinte texto antes de continuar</v>
       </c>
       <c r="W461" s="59"/>
       <c r="X461" s="59"/>
       <c r="Y461" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z461" s="57" t="s">
-        <v>3293</v>
+      <c r="Z461" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N461,""es"",""fr"")"),"Lisez le texte suivant avant de continuer")</f>
+        <v>Lisez le texte suivant avant de continuer</v>
       </c>
       <c r="AA461" s="59"/>
       <c r="AB461" s="59"/>
@@ -39847,7 +39679,7 @@
     </row>
     <row r="462">
       <c r="A462" s="57" t="s">
-        <v>3294</v>
+        <v>3269</v>
       </c>
       <c r="B462" s="57" t="s">
         <v>3242</v>
@@ -39857,8 +39689,21 @@
       </c>
       <c r="D462" s="58"/>
       <c r="E462" s="59"/>
-      <c r="F462" s="57" t="s">
-        <v>3295</v>
+      <c r="F462" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N462,""es"",""ro"")"),"Când utilizați acest proces, puteți solicita informații relevante direct și vă puteți furniza
+Mai multe versiuni actuale pe care le avem.
+Puteți verifica informațiile și alegeți dacă doriți sau nu să le utilizați. Nu sunteți obligat să solicitați informaț"&amp;"iile prin acest serviciu. Dacă acest proces se anulează, veți avea posibilitatea de a
+Completați procesul de căutare și trimiterea de informații manual.
+Rețineți că acest serviciu face parte dintr -un proiect pilot. Selectând „Accept”, el este de acord să"&amp;" participe în mod voluntar la programul pilot. Ar trebui să utilizați doar informațiile pe care le punem la dispoziție pentru a finaliza
+procedură și pentru a verifica dacă procedura a fost finalizată cu succes. Consultați https://www.de4a.eu/aboutproject"&amp;" pentru mai multe detalii.
+")</f>
+        <v>Când utilizați acest proces, puteți solicita informații relevante direct și vă puteți furniza
+Mai multe versiuni actuale pe care le avem.
+Puteți verifica informațiile și alegeți dacă doriți sau nu să le utilizați. Nu sunteți obligat să solicitați informațiile prin acest serviciu. Dacă acest proces se anulează, veți avea posibilitatea de a
+Completați procesul de căutare și trimiterea de informații manual.
+Rețineți că acest serviciu face parte dintr -un proiect pilot. Selectând „Accept”, el este de acord să participe în mod voluntar la programul pilot. Ar trebui să utilizați doar informațiile pe care le punem la dispoziție pentru a finaliza
+procedură și pentru a verifica dacă procedura a fost finalizată cu succes. Consultați https://www.de4a.eu/aboutproject pentru mai multe detalii.
+</v>
       </c>
       <c r="G462" s="59"/>
       <c r="H462" s="59"/>
@@ -39866,7 +39711,7 @@
         <v>0.0</v>
       </c>
       <c r="J462" s="57" t="s">
-        <v>3296</v>
+        <v>3270</v>
       </c>
       <c r="K462" s="59"/>
       <c r="L462" s="59"/>
@@ -39874,31 +39719,70 @@
         <v>1.0</v>
       </c>
       <c r="N462" s="57" t="s">
-        <v>3297</v>
+        <v>3271</v>
       </c>
       <c r="O462" s="59"/>
       <c r="P462" s="59"/>
       <c r="Q462" s="57">
         <v>1.0</v>
       </c>
-      <c r="R462" s="57" t="s">
-        <v>3298</v>
+      <c r="R462" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N462,""es"",""sl"")"),"Ko uporabljate ta postopek, lahko neposredno zahtevate ustrezne informacije in vam zagotovite
+Več trenutne različice imamo.
+Lahko preverite informacije in izberete, ali jih želite uporabiti ali ne. Ne želite zahtevati informacij prek te storitve. Če ta po"&amp;"stopek odpove, boste imeli možnost
+Izpolnite svoj postopek iskanja in pošiljanje informacij ročno.
+Upoštevajte, da je ta storitev del pilotskega projekta. Z izbiro ""Sprejmi"" se strinja, da bo prostovoljno sodeloval v pilotnem programu. Za dokončanje
+pos"&amp;"topek in preveriti, ali je bil postopek uspešno zaključen. Za več podrobnosti glejte https://www.de4a.eu/aboutProject.
+")</f>
+        <v>Ko uporabljate ta postopek, lahko neposredno zahtevate ustrezne informacije in vam zagotovite
+Več trenutne različice imamo.
+Lahko preverite informacije in izberete, ali jih želite uporabiti ali ne. Ne želite zahtevati informacij prek te storitve. Če ta postopek odpove, boste imeli možnost
+Izpolnite svoj postopek iskanja in pošiljanje informacij ročno.
+Upoštevajte, da je ta storitev del pilotskega projekta. Z izbiro "Sprejmi" se strinja, da bo prostovoljno sodeloval v pilotnem programu. Za dokončanje
+postopek in preveriti, ali je bil postopek uspešno zaključen. Za več podrobnosti glejte https://www.de4a.eu/aboutProject.
+</v>
       </c>
       <c r="S462" s="59"/>
       <c r="T462" s="59"/>
       <c r="U462" s="57">
         <v>0.0</v>
       </c>
-      <c r="V462" s="57" t="s">
-        <v>3299</v>
+      <c r="V462" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N462,""es"",""pt"")"),"Ao usar esse processo, você pode solicitar informações relevantes diretamente e fornecer a você o
+Versão mais atual que temos.
+Você pode verificar as informações e escolher se deseja ou não usá -las. Você não é obrigado a solicitar as informações através "&amp;"deste serviço. Se esse processo cancelar, você terá a possibilidade de
+Conclua seu processo procurando e enviando informações manualmente.
+Observe que este serviço faz parte de um projeto piloto. Ao selecionar ""Eu aceito"", ele concorda em participar do "&amp;"programa piloto voluntariamente. Você deve usar apenas as informações que colocamos à sua disposição para concluir o
+procedimento e para verificar se o procedimento foi concluído com sucesso. Consulte https://www.de4a.eu/aboutproject para obter mais detal"&amp;"hes.
+")</f>
+        <v>Ao usar esse processo, você pode solicitar informações relevantes diretamente e fornecer a você o
+Versão mais atual que temos.
+Você pode verificar as informações e escolher se deseja ou não usá -las. Você não é obrigado a solicitar as informações através deste serviço. Se esse processo cancelar, você terá a possibilidade de
+Conclua seu processo procurando e enviando informações manualmente.
+Observe que este serviço faz parte de um projeto piloto. Ao selecionar "Eu aceito", ele concorda em participar do programa piloto voluntariamente. Você deve usar apenas as informações que colocamos à sua disposição para concluir o
+procedimento e para verificar se o procedimento foi concluído com sucesso. Consulte https://www.de4a.eu/aboutproject para obter mais detalhes.
+</v>
       </c>
       <c r="W462" s="59"/>
       <c r="X462" s="59"/>
       <c r="Y462" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z462" s="57" t="s">
-        <v>3300</v>
+      <c r="Z462" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N462,""es"",""fr"")"),"Lorsque vous utilisez ce processus, vous pouvez demander directement des informations pertinentes et vous fournir
+Plus de version actuelle que nous avons.
+Vous pouvez vérifier les informations et choisir si vous souhaitez les utiliser ou non. Vous n'êtes "&amp;"pas obligé de demander les informations via ce service. Si ce processus annule, vous aurez la possibilité de
+Remplissez votre processus à la recherche et à l'envoi d'informations manuellement.
+Notez que ce service fait partie d'un projet pilote. En sélect"&amp;"ionnant ""j'accepte"", il accepte de participer volontairement au programme pilote. Vous devez uniquement utiliser les informations que nous mettons à votre disposition afin de compléter le
+procédure et pour vérifier que la procédure a été achevée avec su"&amp;"ccès. Voir https://www.de4a.eu/aboutproject pour plus de détails.
+")</f>
+        <v>Lorsque vous utilisez ce processus, vous pouvez demander directement des informations pertinentes et vous fournir
+Plus de version actuelle que nous avons.
+Vous pouvez vérifier les informations et choisir si vous souhaitez les utiliser ou non. Vous n'êtes pas obligé de demander les informations via ce service. Si ce processus annule, vous aurez la possibilité de
+Remplissez votre processus à la recherche et à l'envoi d'informations manuellement.
+Notez que ce service fait partie d'un projet pilote. En sélectionnant "j'accepte", il accepte de participer volontairement au programme pilote. Vous devez uniquement utiliser les informations que nous mettons à votre disposition afin de compléter le
+procédure et pour vérifier que la procédure a été achevée avec succès. Voir https://www.de4a.eu/aboutproject pour plus de détails.
+</v>
       </c>
       <c r="AA462" s="59"/>
       <c r="AB462" s="59"/>
@@ -39908,7 +39792,7 @@
     </row>
     <row r="463">
       <c r="A463" s="57" t="s">
-        <v>3301</v>
+        <v>3272</v>
       </c>
       <c r="B463" s="57" t="s">
         <v>3242</v>
@@ -39918,8 +39802,9 @@
       </c>
       <c r="D463" s="58"/>
       <c r="E463" s="59"/>
-      <c r="F463" s="57" t="s">
-        <v>3302</v>
+      <c r="F463" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N463,""es"",""ro"")"),"Dovezi furnizate de")</f>
+        <v>Dovezi furnizate de</v>
       </c>
       <c r="G463" s="59"/>
       <c r="H463" s="59"/>
@@ -39927,7 +39812,7 @@
         <v>0.0</v>
       </c>
       <c r="J463" s="57" t="s">
-        <v>3303</v>
+        <v>3273</v>
       </c>
       <c r="K463" s="59"/>
       <c r="L463" s="59"/>
@@ -39935,31 +39820,34 @@
         <v>1.0</v>
       </c>
       <c r="N463" s="57" t="s">
-        <v>3304</v>
+        <v>3274</v>
       </c>
       <c r="O463" s="59"/>
       <c r="P463" s="59"/>
       <c r="Q463" s="57">
         <v>1.0</v>
       </c>
-      <c r="R463" s="61" t="s">
-        <v>3305</v>
+      <c r="R463" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N463,""es"",""sl"")"),"Dokazi, ki jih predloži")</f>
+        <v>Dokazi, ki jih predloži</v>
       </c>
       <c r="S463" s="59"/>
       <c r="T463" s="59"/>
       <c r="U463" s="57">
         <v>0.0</v>
       </c>
-      <c r="V463" s="57" t="s">
-        <v>3306</v>
+      <c r="V463" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N463,""es"",""pt"")"),"Evidência fornecida por")</f>
+        <v>Evidência fornecida por</v>
       </c>
       <c r="W463" s="59"/>
       <c r="X463" s="59"/>
       <c r="Y463" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z463" s="57" t="s">
-        <v>3307</v>
+      <c r="Z463" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N463,""es"",""fr"")"),"Preuve fournie par")</f>
+        <v>Preuve fournie par</v>
       </c>
       <c r="AA463" s="59"/>
       <c r="AB463" s="59"/>
@@ -39969,7 +39857,7 @@
     </row>
     <row r="464">
       <c r="A464" s="57" t="s">
-        <v>3308</v>
+        <v>3275</v>
       </c>
       <c r="B464" s="57" t="s">
         <v>3242</v>
@@ -39979,8 +39867,9 @@
       </c>
       <c r="D464" s="58"/>
       <c r="E464" s="59"/>
-      <c r="F464" s="57" t="s">
-        <v>3309</v>
+      <c r="F464" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N464,""es"",""ro"")"),"Platforma de intermediere a datelor administrației generale spaniole")</f>
+        <v>Platforma de intermediere a datelor administrației generale spaniole</v>
       </c>
       <c r="G464" s="59"/>
       <c r="H464" s="59"/>
@@ -39988,7 +39877,7 @@
         <v>0.0</v>
       </c>
       <c r="J464" s="57" t="s">
-        <v>3310</v>
+        <v>3276</v>
       </c>
       <c r="K464" s="59"/>
       <c r="L464" s="59"/>
@@ -39996,31 +39885,34 @@
         <v>1.0</v>
       </c>
       <c r="N464" s="57" t="s">
-        <v>3311</v>
+        <v>3277</v>
       </c>
       <c r="O464" s="59"/>
       <c r="P464" s="59"/>
       <c r="Q464" s="57">
         <v>1.0</v>
       </c>
-      <c r="R464" s="61" t="s">
-        <v>3312</v>
+      <c r="R464" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N464,""es"",""sl"")"),"Podatkovni posredniški platformi splošne španske uprave")</f>
+        <v>Podatkovni posredniški platformi splošne španske uprave</v>
       </c>
       <c r="S464" s="59"/>
       <c r="T464" s="59"/>
       <c r="U464" s="57">
         <v>0.0</v>
       </c>
-      <c r="V464" s="57" t="s">
-        <v>3313</v>
+      <c r="V464" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N464,""es"",""pt"")"),"A plataforma de intermediação de dados da administração em espanhol em geral")</f>
+        <v>A plataforma de intermediação de dados da administração em espanhol em geral</v>
       </c>
       <c r="W464" s="59"/>
       <c r="X464" s="59"/>
       <c r="Y464" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z464" s="57" t="s">
-        <v>3314</v>
+      <c r="Z464" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N464,""es"",""fr"")"),"La plate-forme d'intermédiation de données de l'administration d'espagnol générale")</f>
+        <v>La plate-forme d'intermédiation de données de l'administration d'espagnol générale</v>
       </c>
       <c r="AA464" s="59"/>
       <c r="AB464" s="59"/>
@@ -40030,7 +39922,7 @@
     </row>
     <row r="465">
       <c r="A465" s="57" t="s">
-        <v>3315</v>
+        <v>3278</v>
       </c>
       <c r="B465" s="57" t="s">
         <v>3242</v>
@@ -40040,8 +39932,9 @@
       </c>
       <c r="D465" s="58"/>
       <c r="E465" s="59"/>
-      <c r="F465" s="57" t="s">
-        <v>3316</v>
+      <c r="F465" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N465,""es"",""ro"")"),"emit de")</f>
+        <v>emit de</v>
       </c>
       <c r="G465" s="59"/>
       <c r="H465" s="59"/>
@@ -40049,7 +39942,7 @@
         <v>0.0</v>
       </c>
       <c r="J465" s="57" t="s">
-        <v>3317</v>
+        <v>3279</v>
       </c>
       <c r="K465" s="59"/>
       <c r="L465" s="59"/>
@@ -40057,31 +39950,34 @@
         <v>1.0</v>
       </c>
       <c r="N465" s="57" t="s">
-        <v>3318</v>
+        <v>3280</v>
       </c>
       <c r="O465" s="59"/>
       <c r="P465" s="59"/>
       <c r="Q465" s="57">
         <v>1.0</v>
       </c>
-      <c r="R465" s="61" t="s">
-        <v>3319</v>
+      <c r="R465" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N465,""es"",""sl"")"),"oddajati")</f>
+        <v>oddajati</v>
       </c>
       <c r="S465" s="59"/>
       <c r="T465" s="59"/>
       <c r="U465" s="57">
         <v>0.0</v>
       </c>
-      <c r="V465" s="57" t="s">
-        <v>3320</v>
+      <c r="V465" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N465,""es"",""pt"")"),"emitido por")</f>
+        <v>emitido por</v>
       </c>
       <c r="W465" s="59"/>
       <c r="X465" s="59"/>
       <c r="Y465" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z465" s="57" t="s">
-        <v>3321</v>
+      <c r="Z465" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N465,""es"",""fr"")"),"émis par")</f>
+        <v>émis par</v>
       </c>
       <c r="AA465" s="59"/>
       <c r="AB465" s="59"/>
@@ -40091,7 +39987,7 @@
     </row>
     <row r="466">
       <c r="A466" s="57" t="s">
-        <v>3322</v>
+        <v>3281</v>
       </c>
       <c r="B466" s="57" t="s">
         <v>3242</v>
@@ -40101,8 +39997,9 @@
       </c>
       <c r="D466" s="58"/>
       <c r="E466" s="59"/>
-      <c r="F466" s="57" t="s">
-        <v>3323</v>
+      <c r="F466" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N466,""es"",""ro"")"),"Institutul Național de Statistică (INE)")</f>
+        <v>Institutul Național de Statistică (INE)</v>
       </c>
       <c r="G466" s="59"/>
       <c r="H466" s="59"/>
@@ -40110,7 +40007,7 @@
         <v>0.0</v>
       </c>
       <c r="J466" s="57" t="s">
-        <v>3324</v>
+        <v>3282</v>
       </c>
       <c r="K466" s="59"/>
       <c r="L466" s="59"/>
@@ -40118,7 +40015,7 @@
         <v>1.0</v>
       </c>
       <c r="N466" s="57" t="s">
-        <v>3325</v>
+        <v>3283</v>
       </c>
       <c r="O466" s="59"/>
       <c r="P466" s="59"/>
@@ -40126,23 +40023,25 @@
         <v>1.0</v>
       </c>
       <c r="R466" s="57" t="s">
-        <v>3326</v>
+        <v>3284</v>
       </c>
       <c r="S466" s="59"/>
       <c r="T466" s="59"/>
       <c r="U466" s="57">
         <v>0.0</v>
       </c>
-      <c r="V466" s="57" t="s">
-        <v>3327</v>
+      <c r="V466" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N466,""es"",""pt"")"),"Instituto Nacional de Estatísticas (INE)")</f>
+        <v>Instituto Nacional de Estatísticas (INE)</v>
       </c>
       <c r="W466" s="59"/>
       <c r="X466" s="59"/>
       <c r="Y466" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z466" s="57" t="s">
-        <v>3328</v>
+      <c r="Z466" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N466,""es"",""fr"")"),"Institut national des statistiques (INE)")</f>
+        <v>Institut national des statistiques (INE)</v>
       </c>
       <c r="AA466" s="59"/>
       <c r="AB466" s="59"/>
@@ -40152,7 +40051,7 @@
     </row>
     <row r="467">
       <c r="A467" s="57" t="s">
-        <v>3329</v>
+        <v>3285</v>
       </c>
       <c r="B467" s="57" t="s">
         <v>3242</v>
@@ -40162,8 +40061,9 @@
       </c>
       <c r="D467" s="58"/>
       <c r="E467" s="59"/>
-      <c r="F467" s="57" t="s">
-        <v>3330</v>
+      <c r="F467" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N467,""es"",""ro"")"),"Continua")</f>
+        <v>Continua</v>
       </c>
       <c r="G467" s="59"/>
       <c r="H467" s="59"/>
@@ -40171,7 +40071,7 @@
         <v>0.0</v>
       </c>
       <c r="J467" s="57" t="s">
-        <v>3331</v>
+        <v>3286</v>
       </c>
       <c r="K467" s="59"/>
       <c r="L467" s="59"/>
@@ -40179,31 +40079,34 @@
         <v>1.0</v>
       </c>
       <c r="N467" s="57" t="s">
-        <v>3332</v>
+        <v>3287</v>
       </c>
       <c r="O467" s="59"/>
       <c r="P467" s="59"/>
       <c r="Q467" s="57">
         <v>1.0</v>
       </c>
-      <c r="R467" s="57" t="s">
-        <v>3333</v>
+      <c r="R467" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N467,""es"",""sl"")"),"Nadaljevati")</f>
+        <v>Nadaljevati</v>
       </c>
       <c r="S467" s="59"/>
       <c r="T467" s="59"/>
       <c r="U467" s="57">
         <v>0.0</v>
       </c>
-      <c r="V467" s="57" t="s">
-        <v>3334</v>
+      <c r="V467" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N467,""es"",""pt"")"),"Continuar")</f>
+        <v>Continuar</v>
       </c>
       <c r="W467" s="59"/>
       <c r="X467" s="59"/>
       <c r="Y467" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z467" s="57" t="s">
-        <v>3335</v>
+      <c r="Z467" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N467,""es"",""fr"")"),"Procéder")</f>
+        <v>Procéder</v>
       </c>
       <c r="AA467" s="59"/>
       <c r="AB467" s="59"/>
@@ -40213,7 +40116,7 @@
     </row>
     <row r="468">
       <c r="A468" s="57" t="s">
-        <v>3336</v>
+        <v>3288</v>
       </c>
       <c r="B468" s="57" t="s">
         <v>3242</v>
@@ -40223,8 +40126,9 @@
       </c>
       <c r="D468" s="58"/>
       <c r="E468" s="59"/>
-      <c r="F468" s="57" t="s">
-        <v>3330</v>
+      <c r="F468" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N468,""es"",""ro"")"),"Declin")</f>
+        <v>Declin</v>
       </c>
       <c r="G468" s="59"/>
       <c r="H468" s="59"/>
@@ -40232,7 +40136,7 @@
         <v>0.0</v>
       </c>
       <c r="J468" s="57" t="s">
-        <v>3337</v>
+        <v>3289</v>
       </c>
       <c r="K468" s="59"/>
       <c r="L468" s="59"/>
@@ -40240,31 +40144,34 @@
         <v>1.0</v>
       </c>
       <c r="N468" s="57" t="s">
-        <v>3338</v>
+        <v>3290</v>
       </c>
       <c r="O468" s="59"/>
       <c r="P468" s="59"/>
       <c r="Q468" s="57">
         <v>1.0</v>
       </c>
-      <c r="R468" s="57" t="s">
-        <v>3339</v>
+      <c r="R468" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N468,""es"",""sl"")"),"Upad")</f>
+        <v>Upad</v>
       </c>
       <c r="S468" s="59"/>
       <c r="T468" s="59"/>
       <c r="U468" s="57">
         <v>0.0</v>
       </c>
-      <c r="V468" s="57" t="s">
-        <v>3340</v>
+      <c r="V468" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N468,""es"",""pt"")"),"Declínio")</f>
+        <v>Declínio</v>
       </c>
       <c r="W468" s="59"/>
       <c r="X468" s="59"/>
       <c r="Y468" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z468" s="57" t="s">
-        <v>3335</v>
+      <c r="Z468" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N468,""es"",""fr"")"),"Déclin")</f>
+        <v>Déclin</v>
       </c>
       <c r="AA468" s="59"/>
       <c r="AB468" s="59"/>
@@ -40274,7 +40181,7 @@
     </row>
     <row r="469">
       <c r="A469" s="57" t="s">
-        <v>3341</v>
+        <v>3291</v>
       </c>
       <c r="B469" s="57" t="s">
         <v>3242</v>
@@ -40284,8 +40191,9 @@
       </c>
       <c r="D469" s="58"/>
       <c r="E469" s="59"/>
-      <c r="F469" s="57" t="s">
-        <v>3342</v>
+      <c r="F469" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N469,""es"",""ro"")"),"Probele solicitate vor fi trimise următoarei autorități")</f>
+        <v>Probele solicitate vor fi trimise următoarei autorități</v>
       </c>
       <c r="G469" s="59"/>
       <c r="H469" s="59"/>
@@ -40293,7 +40201,7 @@
         <v>0.0</v>
       </c>
       <c r="J469" s="57" t="s">
-        <v>3343</v>
+        <v>3292</v>
       </c>
       <c r="K469" s="59"/>
       <c r="L469" s="59"/>
@@ -40301,31 +40209,34 @@
         <v>1.0</v>
       </c>
       <c r="N469" s="57" t="s">
-        <v>3344</v>
+        <v>3293</v>
       </c>
       <c r="O469" s="59"/>
       <c r="P469" s="59"/>
       <c r="Q469" s="57">
         <v>1.0</v>
       </c>
-      <c r="R469" s="57" t="s">
-        <v>3345</v>
+      <c r="R469" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N469,""es"",""sl"")"),"Zahtevani dokazi bodo poslani naslednjim organom")</f>
+        <v>Zahtevani dokazi bodo poslani naslednjim organom</v>
       </c>
       <c r="S469" s="59"/>
       <c r="T469" s="59"/>
       <c r="U469" s="57">
         <v>0.0</v>
       </c>
-      <c r="V469" s="57" t="s">
-        <v>3346</v>
+      <c r="V469" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N469,""es"",""pt"")"),"A evidência solicitada será enviada para a seguinte autoridade")</f>
+        <v>A evidência solicitada será enviada para a seguinte autoridade</v>
       </c>
       <c r="W469" s="59"/>
       <c r="X469" s="59"/>
       <c r="Y469" s="57">
         <v>0.0</v>
       </c>
-      <c r="Z469" s="57" t="s">
-        <v>3347</v>
+      <c r="Z469" s="57" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(N469,""es"",""fr"")"),"Les preuves demandées seront envoyées à l'autorité suivante")</f>
+        <v>Les preuves demandées seront envoyées à l'autorité suivante</v>
       </c>
       <c r="AA469" s="59"/>
       <c r="AB469" s="59"/>

</xml_diff>